<commit_message>
Refactoring for subgenus-level trees
</commit_message>
<xml_diff>
--- a/tabular/core/flavi-reference_feature_locations.xlsx
+++ b/tabular/core/flavi-reference_feature_locations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flaviviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3404D8-5465-814B-9F68-44D255E36E2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6D86BD-6A79-C54C-9F61-C16183D52965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="500" windowWidth="26680" windowHeight="24820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="128">
   <si>
     <t>featureName</t>
   </si>
@@ -416,6 +416,12 @@
   </si>
   <si>
     <t>NC_027817</t>
+  </si>
+  <si>
+    <t>precursor_polyprotein1</t>
+  </si>
+  <si>
+    <t>precursor_polyprotein2</t>
   </si>
 </sst>
 </file>
@@ -487,7 +493,7 @@
       <name val="Courier"/>
     </font>
   </fonts>
-  <fills count="25">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -632,6 +638,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3101,7 +3113,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3179,6 +3191,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2457">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -5974,10 +5987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1507"/>
+  <dimension ref="A1:H1509"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7755,10 +7768,10 @@
       <c r="E77" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="F77" s="9">
+      <c r="F77" s="27">
         <v>1</v>
       </c>
-      <c r="G77" s="9">
+      <c r="G77" s="27">
         <v>10116</v>
       </c>
     </row>
@@ -7778,10 +7791,10 @@
       <c r="E78" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F78" s="9">
+      <c r="F78" s="27">
         <v>1</v>
       </c>
-      <c r="G78" s="9">
+      <c r="G78" s="27">
         <v>10116</v>
       </c>
     </row>
@@ -7801,10 +7814,10 @@
       <c r="E79" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F79" s="9">
+      <c r="F79" s="27">
         <v>1</v>
       </c>
-      <c r="G79" s="9">
+      <c r="G79" s="27">
         <v>2268</v>
       </c>
     </row>
@@ -7824,10 +7837,10 @@
       <c r="E80" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F80" s="9">
+      <c r="F80" s="27">
         <v>1</v>
       </c>
-      <c r="G80" s="9">
+      <c r="G80" s="27">
         <v>330</v>
       </c>
     </row>
@@ -7847,10 +7860,10 @@
       <c r="E81" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="F81" s="9">
+      <c r="F81" s="27">
         <v>331</v>
       </c>
-      <c r="G81" s="9">
+      <c r="G81" s="27">
         <v>813</v>
       </c>
     </row>
@@ -7870,10 +7883,10 @@
       <c r="E82" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F82" s="9">
+      <c r="F82" s="27">
         <v>589</v>
       </c>
-      <c r="G82" s="9">
+      <c r="G82" s="27">
         <v>813</v>
       </c>
     </row>
@@ -7893,10 +7906,10 @@
       <c r="E83" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="F83" s="9">
+      <c r="F83" s="27">
         <v>814</v>
       </c>
-      <c r="G83" s="9">
+      <c r="G83" s="27">
         <v>2268</v>
       </c>
     </row>
@@ -7916,10 +7929,10 @@
       <c r="E84" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F84" s="9">
+      <c r="F84" s="27">
         <v>2269</v>
       </c>
-      <c r="G84" s="9">
+      <c r="G84" s="27">
         <v>3327</v>
       </c>
     </row>
@@ -7939,10 +7952,10 @@
       <c r="E85" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="F85" s="9">
+      <c r="F85" s="27">
         <v>3328</v>
       </c>
-      <c r="G85" s="9">
+      <c r="G85" s="27">
         <v>4002</v>
       </c>
     </row>
@@ -7962,10 +7975,10 @@
       <c r="E86" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="F86" s="9">
+      <c r="F86" s="27">
         <v>4003</v>
       </c>
-      <c r="G86" s="9">
+      <c r="G86" s="27">
         <v>4392</v>
       </c>
     </row>
@@ -7985,10 +7998,10 @@
       <c r="E87" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F87" s="9">
+      <c r="F87" s="27">
         <v>4393</v>
       </c>
-      <c r="G87" s="9">
+      <c r="G87" s="27">
         <v>6240</v>
       </c>
     </row>
@@ -8008,10 +8021,10 @@
       <c r="E88" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F88" s="9">
+      <c r="F88" s="27">
         <v>6241</v>
       </c>
-      <c r="G88" s="9">
+      <c r="G88" s="27">
         <v>6597</v>
       </c>
     </row>
@@ -8031,10 +8044,10 @@
       <c r="E89" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F89" s="9">
+      <c r="F89" s="27">
         <v>6598</v>
       </c>
-      <c r="G89" s="9">
+      <c r="G89" s="27">
         <v>6666</v>
       </c>
     </row>
@@ -8054,10 +8067,10 @@
       <c r="E90" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F90" s="9">
+      <c r="F90" s="27">
         <v>6667</v>
       </c>
-      <c r="G90" s="9">
+      <c r="G90" s="27">
         <v>7422</v>
       </c>
     </row>
@@ -8077,10 +8090,10 @@
       <c r="E91" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F91" s="9">
+      <c r="F91" s="27">
         <v>7423</v>
       </c>
-      <c r="G91" s="9">
+      <c r="G91" s="27">
         <v>10113</v>
       </c>
     </row>
@@ -8100,10 +8113,10 @@
       <c r="E92" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="F92" s="9">
+      <c r="F92" s="27">
         <v>2269</v>
       </c>
-      <c r="G92" s="9">
+      <c r="G92" s="27">
         <v>10116</v>
       </c>
       <c r="H92" s="27"/>
@@ -8118,16 +8131,16 @@
       <c r="C93" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="D93" s="24" t="s">
+      <c r="D93" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="E93" s="9" t="s">
+      <c r="E93" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="F93" s="1">
+      <c r="F93" s="27">
         <v>1</v>
       </c>
-      <c r="G93" s="1">
+      <c r="G93" s="27">
         <v>10242</v>
       </c>
     </row>
@@ -8141,16 +8154,16 @@
       <c r="C94" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="D94" s="24" t="s">
+      <c r="D94" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="E94" s="9" t="s">
+      <c r="E94" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="F94" s="1">
+      <c r="F94" s="27">
         <v>1</v>
       </c>
-      <c r="G94" s="1">
+      <c r="G94" s="27">
         <v>10242</v>
       </c>
     </row>
@@ -8167,60 +8180,60 @@
       <c r="D95" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="E95" s="9" t="s">
+      <c r="E95" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="F95" s="1">
+      <c r="F95" s="27">
         <v>1</v>
       </c>
-      <c r="G95" s="1">
+      <c r="G95" s="27">
         <v>11434</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B96" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C96" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D96" s="15" t="s">
-        <v>43</v>
+      <c r="A96" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="B96" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="C96" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D96" s="24" t="s">
+        <v>115</v>
       </c>
       <c r="E96" s="27" t="s">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="F96" s="27">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="G96" s="27">
-        <v>10839</v>
+        <v>4197</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B97" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C97" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D97" s="15" t="s">
-        <v>43</v>
+      <c r="A97" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="B97" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="C97" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D97" s="24" t="s">
+        <v>115</v>
       </c>
       <c r="E97" s="27" t="s">
-        <v>15</v>
+        <v>127</v>
       </c>
       <c r="F97" s="27">
-        <v>1</v>
+        <v>4359</v>
       </c>
       <c r="G97" s="27">
-        <v>111</v>
+        <v>10976</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
@@ -8237,13 +8250,13 @@
         <v>43</v>
       </c>
       <c r="E98" s="27" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="F98" s="27">
-        <v>112</v>
+        <v>1</v>
       </c>
       <c r="G98" s="27">
-        <v>10359</v>
+        <v>10839</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
@@ -8260,13 +8273,13 @@
         <v>43</v>
       </c>
       <c r="E99" s="27" t="s">
-        <v>105</v>
+        <v>15</v>
       </c>
       <c r="F99" s="27">
-        <v>112</v>
+        <v>1</v>
       </c>
       <c r="G99" s="27">
-        <v>2436</v>
+        <v>111</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
@@ -8283,13 +8296,13 @@
         <v>43</v>
       </c>
       <c r="E100" s="27" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="F100" s="27">
         <v>112</v>
       </c>
       <c r="G100" s="27">
-        <v>441</v>
+        <v>10359</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -8306,13 +8319,13 @@
         <v>43</v>
       </c>
       <c r="E101" s="27" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="F101" s="27">
-        <v>442</v>
+        <v>112</v>
       </c>
       <c r="G101" s="27">
-        <v>945</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
@@ -8329,13 +8342,13 @@
         <v>43</v>
       </c>
       <c r="E102" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F102" s="27">
-        <v>946</v>
+        <v>112</v>
       </c>
       <c r="G102" s="27">
-        <v>2436</v>
+        <v>441</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
@@ -8352,13 +8365,13 @@
         <v>43</v>
       </c>
       <c r="E103" s="27" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="F103" s="27">
-        <v>2437</v>
+        <v>442</v>
       </c>
       <c r="G103" s="27">
-        <v>10356</v>
+        <v>945</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
@@ -8375,13 +8388,13 @@
         <v>43</v>
       </c>
       <c r="E104" s="27" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="F104" s="27">
-        <v>2437</v>
+        <v>946</v>
       </c>
       <c r="G104" s="27">
-        <v>3495</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
@@ -8398,13 +8411,13 @@
         <v>43</v>
       </c>
       <c r="E105" s="27" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F105" s="27">
-        <v>3496</v>
+        <v>2437</v>
       </c>
       <c r="G105" s="27">
-        <v>4185</v>
+        <v>10356</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
@@ -8421,13 +8434,13 @@
         <v>43</v>
       </c>
       <c r="E106" s="27" t="s">
-        <v>104</v>
+        <v>4</v>
       </c>
       <c r="F106" s="27">
-        <v>4186</v>
+        <v>2437</v>
       </c>
       <c r="G106" s="27">
-        <v>4578</v>
+        <v>3495</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
@@ -8444,13 +8457,13 @@
         <v>43</v>
       </c>
       <c r="E107" s="27" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="F107" s="27">
-        <v>4579</v>
+        <v>3496</v>
       </c>
       <c r="G107" s="27">
-        <v>6444</v>
+        <v>4185</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
@@ -8467,13 +8480,13 @@
         <v>43</v>
       </c>
       <c r="E108" s="27" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="F108" s="27">
-        <v>6445</v>
+        <v>4186</v>
       </c>
       <c r="G108" s="27">
-        <v>6822</v>
+        <v>4578</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
@@ -8490,13 +8503,13 @@
         <v>43</v>
       </c>
       <c r="E109" s="27" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F109" s="27">
-        <v>6823</v>
+        <v>4579</v>
       </c>
       <c r="G109" s="27">
-        <v>6891</v>
+        <v>6444</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
@@ -8513,13 +8526,13 @@
         <v>43</v>
       </c>
       <c r="E110" s="27" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F110" s="27">
-        <v>6892</v>
+        <v>6445</v>
       </c>
       <c r="G110" s="27">
-        <v>7647</v>
+        <v>6822</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
@@ -8536,13 +8549,13 @@
         <v>43</v>
       </c>
       <c r="E111" s="27" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F111" s="27">
-        <v>7648</v>
+        <v>6823</v>
       </c>
       <c r="G111" s="27">
-        <v>10356</v>
+        <v>6891</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
@@ -8559,59 +8572,59 @@
         <v>43</v>
       </c>
       <c r="E112" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="F112" s="27">
+        <v>6892</v>
+      </c>
+      <c r="G112" s="27">
+        <v>7647</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B113" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C113" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D113" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E113" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F113" s="27">
+        <v>7648</v>
+      </c>
+      <c r="G113" s="27">
+        <v>10356</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B114" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C114" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D114" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E114" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F112" s="27">
+      <c r="F114" s="27">
         <v>10357</v>
       </c>
-      <c r="G112" s="27">
+      <c r="G114" s="27">
         <v>10839</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A113" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B113" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C113" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D113" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E113" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F113" s="27">
-        <v>1</v>
-      </c>
-      <c r="G113" s="27">
-        <v>9646</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A114" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B114" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C114" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D114" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E114" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F114" s="27">
-        <v>1</v>
-      </c>
-      <c r="G114" s="27">
-        <v>341</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
@@ -8628,13 +8641,13 @@
         <v>107</v>
       </c>
       <c r="E115" s="27" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="F115" s="27">
-        <v>342</v>
+        <v>1</v>
       </c>
       <c r="G115" s="27">
-        <v>9377</v>
+        <v>9646</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
@@ -8651,13 +8664,13 @@
         <v>107</v>
       </c>
       <c r="E116" s="27" t="s">
-        <v>105</v>
+        <v>15</v>
       </c>
       <c r="F116" s="27">
-        <v>342</v>
+        <v>1</v>
       </c>
       <c r="G116" s="27">
-        <v>2579</v>
+        <v>341</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
@@ -8674,13 +8687,13 @@
         <v>107</v>
       </c>
       <c r="E117" s="27" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="F117" s="27">
         <v>342</v>
       </c>
       <c r="G117" s="27">
-        <v>914</v>
+        <v>9377</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
@@ -8697,13 +8710,13 @@
         <v>107</v>
       </c>
       <c r="E118" s="27" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="F118" s="27">
-        <v>915</v>
+        <v>342</v>
       </c>
       <c r="G118" s="27">
-        <v>1490</v>
+        <v>2579</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
@@ -8720,13 +8733,13 @@
         <v>107</v>
       </c>
       <c r="E119" s="27" t="s">
-        <v>99</v>
+        <v>22</v>
       </c>
       <c r="F119" s="27">
-        <v>1491</v>
+        <v>342</v>
       </c>
       <c r="G119" s="27">
-        <v>2579</v>
+        <v>914</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
@@ -8743,13 +8756,13 @@
         <v>107</v>
       </c>
       <c r="E120" s="27" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F120" s="27">
-        <v>2580</v>
+        <v>915</v>
       </c>
       <c r="G120" s="27">
-        <v>9374</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
@@ -8766,13 +8779,13 @@
         <v>107</v>
       </c>
       <c r="E121" s="27" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F121" s="27">
-        <v>2580</v>
+        <v>1491</v>
       </c>
       <c r="G121" s="27">
-        <v>2768</v>
+        <v>2579</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
@@ -8789,13 +8802,13 @@
         <v>107</v>
       </c>
       <c r="E122" s="27" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F122" s="27">
-        <v>2769</v>
+        <v>2580</v>
       </c>
       <c r="G122" s="27">
-        <v>3419</v>
+        <v>9374</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
@@ -8812,13 +8825,13 @@
         <v>107</v>
       </c>
       <c r="E123" s="27" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="F123" s="27">
-        <v>3420</v>
+        <v>2580</v>
       </c>
       <c r="G123" s="27">
-        <v>5312</v>
+        <v>2768</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
@@ -8835,13 +8848,13 @@
         <v>107</v>
       </c>
       <c r="E124" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F124" s="27">
-        <v>5313</v>
+        <v>2769</v>
       </c>
       <c r="G124" s="27">
-        <v>5474</v>
+        <v>3419</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
@@ -8858,13 +8871,13 @@
         <v>107</v>
       </c>
       <c r="E125" s="27" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="F125" s="27">
-        <v>5475</v>
+        <v>3420</v>
       </c>
       <c r="G125" s="27">
-        <v>6257</v>
+        <v>5312</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
@@ -8881,13 +8894,13 @@
         <v>107</v>
       </c>
       <c r="E126" s="27" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F126" s="27">
-        <v>6258</v>
+        <v>5313</v>
       </c>
       <c r="G126" s="27">
-        <v>9374</v>
+        <v>5474</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
@@ -8904,13 +8917,13 @@
         <v>107</v>
       </c>
       <c r="E127" s="27" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
       <c r="F127" s="27">
-        <v>6258</v>
+        <v>5475</v>
       </c>
       <c r="G127" s="27">
-        <v>7601</v>
+        <v>6257</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
@@ -8927,10 +8940,10 @@
         <v>107</v>
       </c>
       <c r="E128" s="27" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F128" s="27">
-        <v>7602</v>
+        <v>6258</v>
       </c>
       <c r="G128" s="27">
         <v>9374</v>
@@ -8950,55 +8963,59 @@
         <v>107</v>
       </c>
       <c r="E129" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F129" s="27">
+        <v>6258</v>
+      </c>
+      <c r="G129" s="27">
+        <v>7601</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A130" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B130" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C130" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D130" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="E130" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F130" s="27">
+        <v>7602</v>
+      </c>
+      <c r="G130" s="27">
+        <v>9374</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A131" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B131" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C131" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D131" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="E131" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F129" s="27">
+      <c r="F131" s="27">
         <v>9378</v>
       </c>
-      <c r="G129" s="27">
+      <c r="G131" s="27">
         <v>9646</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A130" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B130" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C130" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D130"/>
-      <c r="E130" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F130" s="27">
-        <v>1</v>
-      </c>
-      <c r="G130" s="27">
-        <v>9867</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A131" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B131" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C131" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D131"/>
-      <c r="E131" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F131" s="27">
-        <v>1</v>
-      </c>
-      <c r="G131" s="27">
-        <v>327</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
@@ -9013,13 +9030,13 @@
       </c>
       <c r="D132"/>
       <c r="E132" s="27" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="F132" s="27">
-        <v>328</v>
+        <v>1</v>
       </c>
       <c r="G132" s="27">
-        <v>9501</v>
+        <v>9867</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
@@ -9034,13 +9051,13 @@
       </c>
       <c r="D133"/>
       <c r="E133" s="27" t="s">
-        <v>105</v>
+        <v>15</v>
       </c>
       <c r="F133" s="27">
-        <v>328</v>
+        <v>1</v>
       </c>
       <c r="G133" s="27">
-        <v>2199</v>
+        <v>327</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
@@ -9055,13 +9072,13 @@
       </c>
       <c r="D134"/>
       <c r="E134" s="27" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F134" s="27">
         <v>328</v>
       </c>
       <c r="G134" s="27">
-        <v>564</v>
+        <v>9501</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
@@ -9076,13 +9093,13 @@
       </c>
       <c r="D135"/>
       <c r="E135" s="27" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="F135" s="27">
-        <v>565</v>
+        <v>328</v>
       </c>
       <c r="G135" s="27">
-        <v>1137</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
@@ -9097,13 +9114,13 @@
       </c>
       <c r="D136"/>
       <c r="E136" s="27" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="F136" s="27">
-        <v>1138</v>
+        <v>328</v>
       </c>
       <c r="G136" s="27">
-        <v>2199</v>
+        <v>564</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
@@ -9118,13 +9135,13 @@
       </c>
       <c r="D137"/>
       <c r="E137" s="27" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="F137" s="27">
-        <v>2200</v>
+        <v>565</v>
       </c>
       <c r="G137" s="27">
-        <v>2910</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
@@ -9139,13 +9156,13 @@
       </c>
       <c r="D138"/>
       <c r="E138" s="27" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F138" s="27">
-        <v>2911</v>
+        <v>1138</v>
       </c>
       <c r="G138" s="27">
-        <v>9498</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
@@ -9160,13 +9177,13 @@
       </c>
       <c r="D139"/>
       <c r="E139" s="27" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="F139" s="27">
-        <v>2911</v>
+        <v>2200</v>
       </c>
       <c r="G139" s="27">
-        <v>3630</v>
+        <v>2910</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
@@ -9181,13 +9198,13 @@
       </c>
       <c r="D140"/>
       <c r="E140" s="27" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="F140" s="27">
-        <v>3631</v>
+        <v>2911</v>
       </c>
       <c r="G140" s="27">
-        <v>5514</v>
+        <v>9498</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
@@ -9202,13 +9219,13 @@
       </c>
       <c r="D141"/>
       <c r="E141" s="27" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F141" s="27">
-        <v>5515</v>
+        <v>2911</v>
       </c>
       <c r="G141" s="27">
-        <v>5637</v>
+        <v>3630</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
@@ -9223,13 +9240,13 @@
       </c>
       <c r="D142"/>
       <c r="E142" s="27" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="F142" s="27">
-        <v>5638</v>
+        <v>3631</v>
       </c>
       <c r="G142" s="27">
-        <v>6423</v>
+        <v>5514</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
@@ -9244,13 +9261,13 @@
       </c>
       <c r="D143"/>
       <c r="E143" s="27" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F143" s="27">
-        <v>6424</v>
+        <v>5515</v>
       </c>
       <c r="G143" s="27">
-        <v>9498</v>
+        <v>5637</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
@@ -9265,13 +9282,13 @@
       </c>
       <c r="D144"/>
       <c r="E144" s="27" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
       <c r="F144" s="27">
-        <v>6424</v>
+        <v>5638</v>
       </c>
       <c r="G144" s="27">
-        <v>7797</v>
+        <v>6423</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
@@ -9286,10 +9303,10 @@
       </c>
       <c r="D145"/>
       <c r="E145" s="27" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F145" s="27">
-        <v>7798</v>
+        <v>6424</v>
       </c>
       <c r="G145" s="27">
         <v>9498</v>
@@ -9307,59 +9324,55 @@
       </c>
       <c r="D146"/>
       <c r="E146" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F146" s="27">
+        <v>6424</v>
+      </c>
+      <c r="G146" s="27">
+        <v>7797</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A147" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B147" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C147" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D147"/>
+      <c r="E147" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F147" s="27">
+        <v>7798</v>
+      </c>
+      <c r="G147" s="27">
+        <v>9498</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A148" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B148" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C148" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D148"/>
+      <c r="E148" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F146" s="27">
+      <c r="F148" s="27">
         <v>9502</v>
       </c>
-      <c r="G146" s="27">
+      <c r="G148" s="27">
         <v>9867</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
-        <v>54</v>
-      </c>
-      <c r="B147" t="s">
-        <v>63</v>
-      </c>
-      <c r="C147" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D147" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="E147" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F147" s="27">
-        <v>1</v>
-      </c>
-      <c r="G147" s="27">
-        <v>19199</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
-        <v>54</v>
-      </c>
-      <c r="B148" t="s">
-        <v>63</v>
-      </c>
-      <c r="C148" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D148" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="E148" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F148" s="27">
-        <v>1</v>
-      </c>
-      <c r="G148" s="27">
-        <v>350</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
@@ -9376,13 +9389,13 @@
         <v>110</v>
       </c>
       <c r="E149" s="27" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="F149" s="27">
-        <v>351</v>
+        <v>1</v>
       </c>
       <c r="G149" s="27">
-        <v>18068</v>
+        <v>19199</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
@@ -9399,63 +9412,63 @@
         <v>110</v>
       </c>
       <c r="E150" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F150" s="27">
+        <v>1</v>
+      </c>
+      <c r="G150" s="27">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>54</v>
+      </c>
+      <c r="B151" t="s">
+        <v>63</v>
+      </c>
+      <c r="C151" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D151" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="E151" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F151" s="27">
+        <v>351</v>
+      </c>
+      <c r="G151" s="27">
+        <v>18068</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>54</v>
+      </c>
+      <c r="B152" t="s">
+        <v>63</v>
+      </c>
+      <c r="C152" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D152" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="E152" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F150" s="27">
+      <c r="F152" s="27">
         <v>18069</v>
       </c>
-      <c r="G150" s="27">
+      <c r="G152" s="27">
         <v>19199</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A151" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B151" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="C151" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="D151" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="E151" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F151" s="27">
-        <v>1</v>
-      </c>
-      <c r="G151" s="27">
-        <v>18554</v>
-      </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A152" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="B152" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="C152" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="D152" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="E152" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F152" s="27">
-        <v>1</v>
-      </c>
-      <c r="G152" s="27">
-        <v>199</v>
-      </c>
-    </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A153" s="34" t="s">
+      <c r="A153" s="32" t="s">
         <v>84</v>
       </c>
       <c r="B153" s="32" t="s">
@@ -9468,13 +9481,13 @@
         <v>111</v>
       </c>
       <c r="E153" s="27" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="F153" s="27">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="G153" s="27">
-        <v>17905</v>
+        <v>18554</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
@@ -9491,55 +9504,59 @@
         <v>111</v>
       </c>
       <c r="E154" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F154" s="27">
+        <v>1</v>
+      </c>
+      <c r="G154" s="27">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A155" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B155" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C155" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D155" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E155" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F155" s="27">
+        <v>200</v>
+      </c>
+      <c r="G155" s="27">
+        <v>17905</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A156" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B156" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C156" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D156" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E156" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F154" s="27">
+      <c r="F156" s="27">
         <v>17906</v>
       </c>
-      <c r="G154" s="27">
+      <c r="G156" s="27">
         <v>18554</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A155" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B155" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C155" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D155" s="27"/>
-      <c r="E155" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F155" s="27">
-        <v>1</v>
-      </c>
-      <c r="G155" s="27">
-        <v>12573</v>
-      </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A156" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B156" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C156" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D156" s="27"/>
-      <c r="E156" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F156" s="27">
-        <v>1</v>
-      </c>
-      <c r="G156" s="27">
-        <v>385</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
@@ -9554,13 +9571,13 @@
       </c>
       <c r="D157" s="27"/>
       <c r="E157" s="27" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="F157" s="27">
-        <v>386</v>
+        <v>1</v>
       </c>
       <c r="G157" s="27">
-        <v>12352</v>
+        <v>12573</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
@@ -9575,13 +9592,13 @@
       </c>
       <c r="D158" s="27"/>
       <c r="E158" s="27" t="s">
-        <v>105</v>
+        <v>15</v>
       </c>
       <c r="F158" s="27">
-        <v>386</v>
+        <v>1</v>
       </c>
       <c r="G158" s="27">
-        <v>3583</v>
+        <v>385</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
@@ -9596,13 +9613,13 @@
       </c>
       <c r="D159" s="27"/>
       <c r="E159" s="27" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F159" s="27">
         <v>386</v>
       </c>
       <c r="G159" s="27">
-        <v>889</v>
+        <v>12352</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
@@ -9617,13 +9634,13 @@
       </c>
       <c r="D160" s="27"/>
       <c r="E160" s="27" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="F160" s="27">
-        <v>890</v>
+        <v>386</v>
       </c>
       <c r="G160" s="27">
-        <v>1195</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
@@ -9638,13 +9655,13 @@
       </c>
       <c r="D161" s="27"/>
       <c r="E161" s="27" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="F161" s="27">
-        <v>1196</v>
+        <v>386</v>
       </c>
       <c r="G161" s="27">
-        <v>1876</v>
+        <v>889</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.2">
@@ -9659,13 +9676,13 @@
       </c>
       <c r="D162" s="27"/>
       <c r="E162" s="27" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F162" s="27">
-        <v>1877</v>
+        <v>890</v>
       </c>
       <c r="G162" s="27">
-        <v>2461</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
@@ -9680,13 +9697,13 @@
       </c>
       <c r="D163" s="27"/>
       <c r="E163" s="27" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="F163" s="27">
-        <v>2462</v>
+        <v>1196</v>
       </c>
       <c r="G163" s="27">
-        <v>3583</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
@@ -9701,13 +9718,13 @@
       </c>
       <c r="D164" s="27"/>
       <c r="E164" s="27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F164" s="27">
-        <v>3584</v>
+        <v>1877</v>
       </c>
       <c r="G164" s="27">
-        <v>3793</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
@@ -9722,13 +9739,13 @@
       </c>
       <c r="D165" s="27"/>
       <c r="E165" s="27" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="F165" s="27">
-        <v>3794</v>
+        <v>2462</v>
       </c>
       <c r="G165" s="27">
-        <v>7471</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
@@ -9743,13 +9760,13 @@
       </c>
       <c r="D166" s="27"/>
       <c r="E166" s="27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F166" s="27">
-        <v>7472</v>
+        <v>3584</v>
       </c>
       <c r="G166" s="27">
-        <v>7663</v>
+        <v>3793</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.2">
@@ -9764,13 +9781,13 @@
       </c>
       <c r="D167" s="27"/>
       <c r="E167" s="27" t="s">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="F167" s="27">
-        <v>7664</v>
+        <v>3794</v>
       </c>
       <c r="G167" s="27">
-        <v>8704</v>
+        <v>7471</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.2">
@@ -9785,13 +9802,13 @@
       </c>
       <c r="D168" s="27"/>
       <c r="E168" s="27" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="F168" s="27">
-        <v>8705</v>
+        <v>7472</v>
       </c>
       <c r="G168" s="27">
-        <v>12349</v>
+        <v>7663</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.2">
@@ -9806,13 +9823,13 @@
       </c>
       <c r="D169" s="27"/>
       <c r="E169" s="27" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="F169" s="27">
-        <v>8705</v>
+        <v>7664</v>
       </c>
       <c r="G169" s="27">
-        <v>10192</v>
+        <v>8704</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
@@ -9827,10 +9844,10 @@
       </c>
       <c r="D170" s="27"/>
       <c r="E170" s="27" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F170" s="27">
-        <v>10193</v>
+        <v>8705</v>
       </c>
       <c r="G170" s="27">
         <v>12349</v>
@@ -9848,55 +9865,55 @@
       </c>
       <c r="D171" s="27"/>
       <c r="E171" s="27" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F171" s="27">
-        <v>12360</v>
+        <v>8705</v>
       </c>
       <c r="G171" s="27">
-        <v>12573</v>
+        <v>10192</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A172" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B172" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C172" s="27" t="s">
-        <v>57</v>
+      <c r="A172" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B172" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C172" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D172" s="27"/>
       <c r="E172" s="27" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="F172" s="27">
-        <v>1</v>
+        <v>10193</v>
       </c>
       <c r="G172" s="27">
-        <v>10053</v>
+        <v>12349</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A173" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B173" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C173" s="27" t="s">
-        <v>57</v>
+      <c r="A173" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B173" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C173" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D173" s="27"/>
       <c r="E173" s="27" t="s">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="F173" s="27">
-        <v>1</v>
+        <v>12360</v>
       </c>
       <c r="G173" s="27">
-        <v>10053</v>
+        <v>12573</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.2">
@@ -9911,13 +9928,13 @@
       </c>
       <c r="D174" s="27"/>
       <c r="E174" s="27" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="F174" s="27">
         <v>1</v>
       </c>
       <c r="G174" s="27">
-        <v>2358</v>
+        <v>10053</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.2">
@@ -9932,13 +9949,13 @@
       </c>
       <c r="D175" s="27"/>
       <c r="E175" s="27" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="F175" s="27">
         <v>1</v>
       </c>
       <c r="G175" s="27">
-        <v>345</v>
+        <v>10053</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.2">
@@ -9953,13 +9970,13 @@
       </c>
       <c r="D176" s="27"/>
       <c r="E176" s="27" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="F176" s="27">
-        <v>346</v>
+        <v>1</v>
       </c>
       <c r="G176" s="27">
-        <v>852</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
@@ -9974,13 +9991,13 @@
       </c>
       <c r="D177" s="27"/>
       <c r="E177" s="27" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="F177" s="27">
-        <v>655</v>
+        <v>1</v>
       </c>
       <c r="G177" s="27">
-        <v>852</v>
+        <v>345</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
@@ -9995,13 +10012,13 @@
       </c>
       <c r="D178" s="27"/>
       <c r="E178" s="27" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="F178" s="27">
-        <v>853</v>
+        <v>346</v>
       </c>
       <c r="G178" s="27">
-        <v>2358</v>
+        <v>852</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
@@ -10016,13 +10033,13 @@
       </c>
       <c r="D179" s="27"/>
       <c r="E179" s="27" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="F179" s="27">
-        <v>2359</v>
+        <v>655</v>
       </c>
       <c r="G179" s="27">
-        <v>10050</v>
+        <v>852</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
@@ -10037,13 +10054,13 @@
       </c>
       <c r="D180" s="27"/>
       <c r="E180" s="27" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="F180" s="27">
-        <v>2359</v>
+        <v>853</v>
       </c>
       <c r="G180" s="27">
-        <v>3390</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
@@ -10058,13 +10075,13 @@
       </c>
       <c r="D181" s="27"/>
       <c r="E181" s="27" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F181" s="27">
-        <v>3391</v>
+        <v>2359</v>
       </c>
       <c r="G181" s="27">
-        <v>3978</v>
+        <v>10050</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
@@ -10079,13 +10096,13 @@
       </c>
       <c r="D182" s="27"/>
       <c r="E182" s="27" t="s">
-        <v>104</v>
+        <v>4</v>
       </c>
       <c r="F182" s="27">
-        <v>3979</v>
+        <v>2359</v>
       </c>
       <c r="G182" s="27">
-        <v>4431</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
@@ -10100,13 +10117,13 @@
       </c>
       <c r="D183" s="27"/>
       <c r="E183" s="27" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="F183" s="27">
-        <v>4432</v>
+        <v>3391</v>
       </c>
       <c r="G183" s="27">
-        <v>6303</v>
+        <v>3978</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
@@ -10121,13 +10138,13 @@
       </c>
       <c r="D184" s="27"/>
       <c r="E184" s="27" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="F184" s="27">
-        <v>6304</v>
+        <v>3979</v>
       </c>
       <c r="G184" s="27">
-        <v>6687</v>
+        <v>4431</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
@@ -10142,13 +10159,13 @@
       </c>
       <c r="D185" s="27"/>
       <c r="E185" s="27" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F185" s="27">
-        <v>6688</v>
+        <v>4432</v>
       </c>
       <c r="G185" s="27">
-        <v>6762</v>
+        <v>6303</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
@@ -10163,13 +10180,13 @@
       </c>
       <c r="D186" s="27"/>
       <c r="E186" s="27" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F186" s="27">
-        <v>6763</v>
+        <v>6304</v>
       </c>
       <c r="G186" s="27">
-        <v>7557</v>
+        <v>6687</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
@@ -10184,55 +10201,57 @@
       </c>
       <c r="D187" s="27"/>
       <c r="E187" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F187" s="27">
+        <v>6688</v>
+      </c>
+      <c r="G187" s="27">
+        <v>6762</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A188" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B188" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C188" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D188" s="27"/>
+      <c r="E188" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="F188" s="27">
+        <v>6763</v>
+      </c>
+      <c r="G188" s="27">
+        <v>7557</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A189" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B189" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C189" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D189" s="27"/>
+      <c r="E189" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="F187" s="27">
+      <c r="F189" s="27">
         <v>7558</v>
       </c>
-      <c r="G187" s="27">
+      <c r="G189" s="27">
         <v>10050</v>
       </c>
-      <c r="H187" s="25"/>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A188" t="s">
-        <v>118</v>
-      </c>
-      <c r="B188" t="s">
-        <v>119</v>
-      </c>
-      <c r="C188" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="E188" t="s">
-        <v>83</v>
-      </c>
-      <c r="F188">
-        <v>1</v>
-      </c>
-      <c r="G188">
-        <v>5938</v>
-      </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A189" t="s">
-        <v>118</v>
-      </c>
-      <c r="B189" t="s">
-        <v>119</v>
-      </c>
-      <c r="C189" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="E189" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="F189" s="27">
-        <v>117</v>
-      </c>
-      <c r="G189" s="27">
-        <v>2543</v>
-      </c>
+      <c r="H189" s="25"/>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
@@ -10244,30 +10263,60 @@
       <c r="C190" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="E190" s="27" t="s">
+      <c r="E190" t="s">
+        <v>83</v>
+      </c>
+      <c r="F190">
+        <v>1</v>
+      </c>
+      <c r="G190">
+        <v>5938</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>118</v>
+      </c>
+      <c r="B191" t="s">
+        <v>119</v>
+      </c>
+      <c r="C191" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="E191" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="F191" s="27">
+        <v>117</v>
+      </c>
+      <c r="G191" s="27">
+        <v>2543</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>118</v>
+      </c>
+      <c r="B192" t="s">
+        <v>119</v>
+      </c>
+      <c r="C192" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="E192" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="F190">
-        <f t="shared" ref="F190" si="0">(D190+2824)</f>
+      <c r="F192">
+        <f t="shared" ref="F192" si="0">(D192+2824)</f>
         <v>2824</v>
       </c>
-      <c r="G190" s="27">
+      <c r="G192" s="27">
         <v>5673</v>
       </c>
-    </row>
-    <row r="229" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B229" s="1"/>
-      <c r="C229" s="5"/>
-    </row>
-    <row r="230" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B230" s="1"/>
-      <c r="C230" s="5"/>
-      <c r="D230" s="5"/>
     </row>
     <row r="231" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B231" s="1"/>
       <c r="C231" s="5"/>
-      <c r="D231" s="5"/>
     </row>
     <row r="232" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B232" s="1"/>
@@ -10376,21 +10425,21 @@
     </row>
     <row r="253" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B253" s="1"/>
+      <c r="C253" s="5"/>
       <c r="D253" s="5"/>
     </row>
     <row r="254" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B254" s="1"/>
       <c r="C254" s="5"/>
+      <c r="D254" s="5"/>
     </row>
     <row r="255" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B255" s="1"/>
-      <c r="C255" s="5"/>
       <c r="D255" s="5"/>
     </row>
     <row r="256" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B256" s="1"/>
       <c r="C256" s="5"/>
-      <c r="D256" s="5"/>
     </row>
     <row r="257" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B257" s="1"/>
@@ -10413,22 +10462,26 @@
       <c r="D260" s="5"/>
     </row>
     <row r="261" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B261" s="1"/>
+      <c r="C261" s="5"/>
       <c r="D261" s="5"/>
     </row>
-    <row r="943" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E943" s="1"/>
-    </row>
-    <row r="1079" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1079" s="1"/>
-    </row>
-    <row r="1080" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1080" s="1"/>
-    </row>
-    <row r="1205" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1205" s="1"/>
-    </row>
-    <row r="1206" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1206" s="1"/>
+    <row r="262" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B262" s="1"/>
+      <c r="C262" s="5"/>
+      <c r="D262" s="5"/>
+    </row>
+    <row r="263" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D263" s="5"/>
+    </row>
+    <row r="945" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E945" s="1"/>
+    </row>
+    <row r="1081" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1081" s="1"/>
+    </row>
+    <row r="1082" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1082" s="1"/>
     </row>
     <row r="1207" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1207" s="1"/>
@@ -10442,23 +10495,23 @@
     <row r="1210" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1210" s="1"/>
     </row>
-    <row r="1255" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E1255" s="1"/>
-      <c r="F1255" s="1"/>
-    </row>
-    <row r="1256" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E1256" s="1"/>
-      <c r="F1256" s="1"/>
+    <row r="1211" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1211" s="1"/>
+    </row>
+    <row r="1212" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1212" s="1"/>
     </row>
     <row r="1257" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E1257" s="1"/>
       <c r="F1257" s="1"/>
     </row>
+    <row r="1258" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E1258" s="1"/>
+      <c r="F1258" s="1"/>
+    </row>
     <row r="1259" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1259" s="1"/>
-    </row>
-    <row r="1260" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1260" s="1"/>
+      <c r="E1259" s="1"/>
+      <c r="F1259" s="1"/>
     </row>
     <row r="1261" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1261" s="1"/>
@@ -10469,11 +10522,11 @@
     <row r="1263" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1263" s="1"/>
     </row>
-    <row r="1282" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1282" s="1"/>
-    </row>
-    <row r="1283" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1283" s="1"/>
+    <row r="1264" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1264" s="1"/>
+    </row>
+    <row r="1265" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1265" s="1"/>
     </row>
     <row r="1284" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1284" s="1"/>
@@ -10490,12 +10543,12 @@
     <row r="1288" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1288" s="1"/>
     </row>
+    <row r="1289" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1289" s="1"/>
+    </row>
     <row r="1290" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1290" s="1"/>
     </row>
-    <row r="1291" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1291" s="1"/>
-    </row>
     <row r="1292" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1292" s="1"/>
     </row>
@@ -10508,11 +10561,11 @@
     <row r="1295" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1295" s="1"/>
     </row>
-    <row r="1347" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1347" s="1"/>
-    </row>
-    <row r="1348" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1348" s="1"/>
+    <row r="1296" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1296" s="1"/>
+    </row>
+    <row r="1297" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1297" s="1"/>
     </row>
     <row r="1349" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1349" s="1"/>
@@ -10520,23 +10573,23 @@
     <row r="1350" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1350" s="1"/>
     </row>
+    <row r="1351" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1351" s="1"/>
+    </row>
     <row r="1352" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1352" s="1"/>
     </row>
-    <row r="1353" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1353" s="1"/>
-    </row>
     <row r="1354" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1354" s="1"/>
     </row>
     <row r="1355" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1355" s="1"/>
     </row>
-    <row r="1390" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1390" s="1"/>
-    </row>
-    <row r="1391" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1391" s="1"/>
+    <row r="1356" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1356" s="1"/>
+    </row>
+    <row r="1357" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1357" s="1"/>
     </row>
     <row r="1392" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1392" s="1"/>
@@ -10550,37 +10603,37 @@
     <row r="1395" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1395" s="1"/>
     </row>
-    <row r="1437" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E1437" s="1"/>
-      <c r="F1437" s="1"/>
-    </row>
-    <row r="1438" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C1438" s="6"/>
-      <c r="E1438" s="1"/>
-      <c r="F1438" s="1"/>
+    <row r="1396" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1396" s="1"/>
+    </row>
+    <row r="1397" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1397" s="1"/>
     </row>
     <row r="1439" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C1439" s="6"/>
-      <c r="D1439" s="6"/>
       <c r="E1439" s="1"/>
       <c r="F1439" s="1"/>
     </row>
     <row r="1440" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C1440" s="6"/>
-      <c r="D1440" s="6"/>
       <c r="E1440" s="1"/>
       <c r="F1440" s="1"/>
     </row>
-    <row r="1441" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="1441" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C1441" s="6"/>
       <c r="D1441" s="6"/>
       <c r="E1441" s="1"/>
       <c r="F1441" s="1"/>
     </row>
-    <row r="1504" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1504" s="1"/>
-    </row>
-    <row r="1505" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1505" s="1"/>
+    <row r="1442" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C1442" s="6"/>
+      <c r="D1442" s="6"/>
+      <c r="E1442" s="1"/>
+      <c r="F1442" s="1"/>
+    </row>
+    <row r="1443" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D1443" s="6"/>
+      <c r="E1443" s="1"/>
+      <c r="F1443" s="1"/>
     </row>
     <row r="1506" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1506" s="1"/>
@@ -10588,10 +10641,16 @@
     <row r="1507" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1507" s="1"/>
     </row>
+    <row r="1508" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1508" s="1"/>
+    </row>
+    <row r="1509" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1509" s="1"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G1460">
-    <sortCondition ref="C2:C1460"/>
-    <sortCondition ref="D2:D1460"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G1462">
+    <sortCondition ref="C2:C1462"/>
+    <sortCondition ref="D2:D1462"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added feature locations (basic) for new reference sequences
</commit_message>
<xml_diff>
--- a/tabular/core/flavi-reference_feature_locations.xlsx
+++ b/tabular/core/flavi-reference_feature_locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/RNA/Flavivirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F175AF-CA37-2045-B853-C296F4E739A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE26BE1-D72C-DD4F-92A8-9C0263FF45A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="166">
   <si>
     <t>featureName</t>
   </si>
@@ -350,9 +350,6 @@
     <t>non_structural_proteins</t>
   </si>
   <si>
-    <t>Primate</t>
-  </si>
-  <si>
     <t>NC_024113</t>
   </si>
   <si>
@@ -435,13 +432,118 @@
   </si>
   <si>
     <t>REF_PESTI_1_BVDV1</t>
+  </si>
+  <si>
+    <t>REF_HEPACI_2_HCV_L</t>
+  </si>
+  <si>
+    <t>NC_031916</t>
+  </si>
+  <si>
+    <t>Hepaci1</t>
+  </si>
+  <si>
+    <t>Hepaci2</t>
+  </si>
+  <si>
+    <t>NC_038430</t>
+  </si>
+  <si>
+    <t>REF_HEPACI_3_HCV_K</t>
+  </si>
+  <si>
+    <t>Hepaci3</t>
+  </si>
+  <si>
+    <t>Hepaci4</t>
+  </si>
+  <si>
+    <t>REF_HEPACI_4_HCV_J</t>
+  </si>
+  <si>
+    <t>NC_038429</t>
+  </si>
+  <si>
+    <t>REF_HEPACI_5_BEHV</t>
+  </si>
+  <si>
+    <t>MN062427</t>
+  </si>
+  <si>
+    <t>MT371439</t>
+  </si>
+  <si>
+    <t>REF_HEPACI_7_WHCV</t>
+  </si>
+  <si>
+    <t>REF_HEPACI_6_GHV</t>
+  </si>
+  <si>
+    <t>Hepaci5</t>
+  </si>
+  <si>
+    <t>Hepaci6</t>
+  </si>
+  <si>
+    <t>Hepaci7</t>
+  </si>
+  <si>
+    <t>MG599993</t>
+  </si>
+  <si>
+    <t>REF_HEPACI_8_WmeHCV</t>
+  </si>
+  <si>
+    <t>Hepaci8</t>
+  </si>
+  <si>
+    <t>REF_HEPACI_9_WLSV</t>
+  </si>
+  <si>
+    <t>Hepaci9</t>
+  </si>
+  <si>
+    <t>NC_028377</t>
+  </si>
+  <si>
+    <t>MG599990</t>
+  </si>
+  <si>
+    <t>REF_PESTI_2_NrPeV</t>
+  </si>
+  <si>
+    <t>Pesti1</t>
+  </si>
+  <si>
+    <t>Pesti2</t>
+  </si>
+  <si>
+    <t>Pesti3</t>
+  </si>
+  <si>
+    <t>Pesti4</t>
+  </si>
+  <si>
+    <t>NC_025677</t>
+  </si>
+  <si>
+    <t>REF_PESTI_3_APPeV</t>
+  </si>
+  <si>
+    <t>REF_PESTI_4_NdsPV</t>
+  </si>
+  <si>
+    <t>MG599984</t>
+  </si>
+  <si>
+    <t>NC_038964</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -513,8 +615,14 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="27">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -671,6 +779,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3140,7 +3254,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3211,6 +3325,9 @@
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2457">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -6013,10 +6130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1504"/>
+  <dimension ref="A1:H1526"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B162" sqref="A1:G191"/>
+    <sheetView tabSelected="1" topLeftCell="A169" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E177" sqref="A1:G213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6455,7 +6572,7 @@
         <v>14</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>79</v>
@@ -6478,7 +6595,7 @@
         <v>14</v>
       </c>
       <c r="D20" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>15</v>
@@ -6501,7 +6618,7 @@
         <v>14</v>
       </c>
       <c r="D21" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>66</v>
@@ -6524,7 +6641,7 @@
         <v>14</v>
       </c>
       <c r="D22" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>101</v>
@@ -6547,7 +6664,7 @@
         <v>14</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>90</v>
@@ -6570,7 +6687,7 @@
         <v>14</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>67</v>
@@ -6593,7 +6710,7 @@
         <v>14</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>91</v>
@@ -6616,7 +6733,7 @@
         <v>14</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>4</v>
@@ -6639,7 +6756,7 @@
         <v>14</v>
       </c>
       <c r="D27" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>99</v>
@@ -6662,7 +6779,7 @@
         <v>14</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>100</v>
@@ -6685,7 +6802,7 @@
         <v>14</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>7</v>
@@ -6708,7 +6825,7 @@
         <v>14</v>
       </c>
       <c r="D30" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>86</v>
@@ -6731,7 +6848,7 @@
         <v>14</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>19</v>
@@ -6754,7 +6871,7 @@
         <v>14</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>92</v>
@@ -6777,7 +6894,7 @@
         <v>14</v>
       </c>
       <c r="D33" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>10</v>
@@ -6800,7 +6917,7 @@
         <v>14</v>
       </c>
       <c r="D34" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>102</v>
@@ -8405,13 +8522,13 @@
         <v>34</v>
       </c>
       <c r="B104" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C104" s="28" t="s">
         <v>21</v>
       </c>
       <c r="D104" s="36" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="E104" s="24" t="s">
         <v>79</v>
@@ -8428,13 +8545,13 @@
         <v>34</v>
       </c>
       <c r="B105" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C105" s="28" t="s">
         <v>21</v>
       </c>
       <c r="D105" s="36" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="E105" s="24" t="s">
         <v>15</v>
@@ -8451,13 +8568,13 @@
         <v>34</v>
       </c>
       <c r="B106" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C106" s="28" t="s">
         <v>21</v>
       </c>
       <c r="D106" s="36" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="E106" s="24" t="s">
         <v>66</v>
@@ -8474,13 +8591,13 @@
         <v>34</v>
       </c>
       <c r="B107" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C107" s="28" t="s">
         <v>21</v>
       </c>
       <c r="D107" s="36" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="E107" s="24" t="s">
         <v>101</v>
@@ -8497,13 +8614,13 @@
         <v>34</v>
       </c>
       <c r="B108" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C108" s="28" t="s">
         <v>21</v>
       </c>
       <c r="D108" s="36" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="E108" s="24" t="s">
         <v>22</v>
@@ -8520,13 +8637,13 @@
         <v>34</v>
       </c>
       <c r="B109" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C109" s="28" t="s">
         <v>21</v>
       </c>
       <c r="D109" s="36" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="E109" s="24" t="s">
         <v>94</v>
@@ -8543,13 +8660,13 @@
         <v>34</v>
       </c>
       <c r="B110" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C110" s="28" t="s">
         <v>21</v>
       </c>
       <c r="D110" s="36" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="E110" s="24" t="s">
         <v>95</v>
@@ -8566,13 +8683,13 @@
         <v>34</v>
       </c>
       <c r="B111" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C111" s="28" t="s">
         <v>21</v>
       </c>
       <c r="D111" s="36" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="E111" s="24" t="s">
         <v>102</v>
@@ -8589,13 +8706,13 @@
         <v>34</v>
       </c>
       <c r="B112" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C112" s="28" t="s">
         <v>21</v>
       </c>
       <c r="D112" s="36" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="E112" s="24" t="s">
         <v>93</v>
@@ -8612,13 +8729,13 @@
         <v>34</v>
       </c>
       <c r="B113" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C113" s="28" t="s">
         <v>21</v>
       </c>
       <c r="D113" s="36" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="E113" s="24" t="s">
         <v>98</v>
@@ -8635,13 +8752,13 @@
         <v>34</v>
       </c>
       <c r="B114" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C114" s="28" t="s">
         <v>21</v>
       </c>
       <c r="D114" s="36" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="E114" s="24" t="s">
         <v>7</v>
@@ -8658,13 +8775,13 @@
         <v>34</v>
       </c>
       <c r="B115" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C115" s="28" t="s">
         <v>21</v>
       </c>
       <c r="D115" s="36" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="E115" s="24" t="s">
         <v>96</v>
@@ -8681,13 +8798,13 @@
         <v>34</v>
       </c>
       <c r="B116" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C116" s="28" t="s">
         <v>21</v>
       </c>
       <c r="D116" s="36" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="E116" s="24" t="s">
         <v>97</v>
@@ -8704,13 +8821,13 @@
         <v>34</v>
       </c>
       <c r="B117" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C117" s="28" t="s">
         <v>21</v>
       </c>
       <c r="D117" s="36" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="E117" s="24" t="s">
         <v>10</v>
@@ -8727,13 +8844,13 @@
         <v>34</v>
       </c>
       <c r="B118" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C118" s="28" t="s">
         <v>21</v>
       </c>
       <c r="D118" s="36" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="E118" s="24" t="s">
         <v>24</v>
@@ -8750,13 +8867,13 @@
         <v>34</v>
       </c>
       <c r="B119" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C119" s="28" t="s">
         <v>21</v>
       </c>
       <c r="D119" s="36" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="E119" s="24" t="s">
         <v>25</v>
@@ -8773,13 +8890,13 @@
         <v>34</v>
       </c>
       <c r="B120" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C120" s="28" t="s">
         <v>21</v>
       </c>
       <c r="D120" s="36" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="E120" s="24" t="s">
         <v>11</v>
@@ -8792,16 +8909,18 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A121" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B121" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="C121" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D121"/>
+      <c r="A121" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="B121" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="C121" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D121" s="49" t="s">
+        <v>134</v>
+      </c>
       <c r="E121" s="24" t="s">
         <v>79</v>
       </c>
@@ -8809,322 +8928,352 @@
         <v>1</v>
       </c>
       <c r="G121" s="24">
-        <v>9867</v>
+        <v>8916</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A122" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B122" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="C122" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D122"/>
+      <c r="A122" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="B122" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="C122" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D122" s="49" t="s">
+        <v>134</v>
+      </c>
       <c r="E122" s="24" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="F122" s="24">
+        <v>174</v>
+      </c>
+      <c r="G122" s="24">
+        <v>8879</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A123" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="B123" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="C123" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D123" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="E123" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F123" s="24">
         <v>1</v>
       </c>
-      <c r="G122" s="24">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A123" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B123" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="C123" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D123"/>
-      <c r="E123" s="24" t="s">
+      <c r="G123" s="24">
+        <v>9609</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A124" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="B124" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="C124" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D124" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="E124" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="F123" s="24">
-        <v>328</v>
-      </c>
-      <c r="G123" s="24">
-        <v>9501</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A124" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B124" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="C124" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D124"/>
-      <c r="E124" s="24" t="s">
-        <v>101</v>
-      </c>
       <c r="F124" s="24">
-        <v>328</v>
+        <v>281</v>
       </c>
       <c r="G124" s="24">
-        <v>2199</v>
+        <v>9355</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A125" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B125" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="C125" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D125"/>
+      <c r="A125" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="B125" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="C125" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D125" s="49" t="s">
+        <v>138</v>
+      </c>
       <c r="E125" s="24" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="F125" s="24">
-        <v>328</v>
+        <v>1</v>
       </c>
       <c r="G125" s="24">
-        <v>564</v>
+        <v>9687</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A126" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B126" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="C126" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D126"/>
+      <c r="A126" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="B126" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="C126" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D126" s="49" t="s">
+        <v>138</v>
+      </c>
       <c r="E126" s="24" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="F126" s="24">
-        <v>565</v>
+        <v>558</v>
       </c>
       <c r="G126" s="24">
-        <v>1137</v>
+        <v>9602</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A127" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B127" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="C127" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D127"/>
+      <c r="A127" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="B127" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="C127" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D127" s="49" t="s">
+        <v>146</v>
+      </c>
       <c r="E127" s="24" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="F127" s="24">
-        <v>1138</v>
+        <v>1</v>
       </c>
       <c r="G127" s="24">
-        <v>2199</v>
+        <v>11013</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A128" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B128" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="C128" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D128"/>
+      <c r="A128" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="B128" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="C128" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D128" s="49" t="s">
+        <v>146</v>
+      </c>
       <c r="E128" s="24" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F128" s="24">
-        <v>2200</v>
+        <v>578</v>
       </c>
       <c r="G128" s="24">
-        <v>2910</v>
+        <v>10870</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A129" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B129" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="C129" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D129"/>
+      <c r="A129" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="B129" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="C129" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D129" s="49" t="s">
+        <v>147</v>
+      </c>
       <c r="E129" s="24" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="F129" s="24">
-        <v>2911</v>
+        <v>1</v>
       </c>
       <c r="G129" s="24">
-        <v>9498</v>
+        <v>10199</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A130" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B130" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="C130" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D130"/>
+      <c r="A130" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="B130" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="C130" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D130" s="49" t="s">
+        <v>147</v>
+      </c>
       <c r="E130" s="24" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="F130" s="24">
-        <v>2911</v>
+        <v>3</v>
       </c>
       <c r="G130" s="24">
-        <v>3630</v>
+        <v>10127</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A131" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B131" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="C131" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D131"/>
+      <c r="A131" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="B131" s="48" t="s">
+        <v>144</v>
+      </c>
+      <c r="C131" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D131" s="49" t="s">
+        <v>148</v>
+      </c>
       <c r="E131" s="24" t="s">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="F131" s="24">
-        <v>3631</v>
+        <v>1</v>
       </c>
       <c r="G131" s="24">
-        <v>5514</v>
+        <v>10272</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A132" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B132" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="C132" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D132"/>
+      <c r="A132" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="B132" s="48" t="s">
+        <v>144</v>
+      </c>
+      <c r="C132" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D132" s="49" t="s">
+        <v>148</v>
+      </c>
       <c r="E132" s="24" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="F132" s="24">
-        <v>5515</v>
+        <v>174</v>
       </c>
       <c r="G132" s="24">
-        <v>5637</v>
+        <v>10241</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A133" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B133" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="C133" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D133"/>
+      <c r="A133" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="B133" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="C133" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D133" s="49" t="s">
+        <v>151</v>
+      </c>
       <c r="E133" s="24" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F133" s="24">
-        <v>5638</v>
+        <v>1</v>
       </c>
       <c r="G133" s="24">
-        <v>6423</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A134" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B134" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="C134" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D134"/>
+        <v>8697</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="17" x14ac:dyDescent="0.25">
+      <c r="A134" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="B134" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="C134" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D134" s="49" t="s">
+        <v>151</v>
+      </c>
       <c r="E134" s="24" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="F134" s="24">
-        <v>6424</v>
-      </c>
-      <c r="G134" s="24">
-        <v>9498</v>
+        <v>1</v>
+      </c>
+      <c r="G134" s="50">
+        <v>8622</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A135" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B135" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="C135" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D135"/>
+      <c r="A135" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="B135" s="48" t="s">
+        <v>152</v>
+      </c>
+      <c r="C135" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D135" s="49" t="s">
+        <v>153</v>
+      </c>
       <c r="E135" s="24" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="F135" s="24">
-        <v>6424</v>
+        <v>1</v>
       </c>
       <c r="G135" s="24">
-        <v>7797</v>
+        <v>9653</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A136" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B136" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="C136" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D136"/>
+      <c r="A136" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="B136" s="48" t="s">
+        <v>152</v>
+      </c>
+      <c r="C136" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D136" s="49" t="s">
+        <v>153</v>
+      </c>
       <c r="E136" s="24" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="F136" s="24">
-        <v>7798</v>
+        <v>132</v>
       </c>
       <c r="G136" s="24">
-        <v>9498</v>
+        <v>9392</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
@@ -9132,51 +9281,51 @@
         <v>37</v>
       </c>
       <c r="B137" s="32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C137" s="32" t="s">
         <v>26</v>
       </c>
       <c r="D137"/>
       <c r="E137" s="24" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="F137" s="24">
-        <v>9502</v>
+        <v>1</v>
       </c>
       <c r="G137" s="24">
         <v>9867</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A138" s="47" t="s">
-        <v>127</v>
-      </c>
-      <c r="B138" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="C138" s="47" t="s">
+      <c r="A138" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B138" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C138" s="32" t="s">
         <v>26</v>
       </c>
       <c r="D138"/>
       <c r="E138" s="24" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="F138" s="24">
         <v>1</v>
       </c>
       <c r="G138" s="24">
-        <v>10479</v>
+        <v>327</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A139" s="47" t="s">
-        <v>127</v>
-      </c>
-      <c r="B139" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="C139" s="47" t="s">
+      <c r="A139" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B139" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C139" s="32" t="s">
         <v>26</v>
       </c>
       <c r="D139"/>
@@ -9184,614 +9333,614 @@
         <v>66</v>
       </c>
       <c r="F139" s="24">
-        <v>618</v>
+        <v>328</v>
       </c>
       <c r="G139" s="24">
-        <v>10187</v>
+        <v>9501</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A140" s="47" t="s">
-        <v>127</v>
-      </c>
-      <c r="B140" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="C140" s="47" t="s">
+      <c r="A140" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B140" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C140" s="32" t="s">
         <v>26</v>
       </c>
       <c r="D140"/>
       <c r="E140" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F140" s="24">
+        <v>328</v>
+      </c>
+      <c r="G140" s="24">
+        <v>2199</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A141" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B141" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="F140" s="24">
-        <v>618</v>
-      </c>
-      <c r="G140" s="24">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A141" s="47" t="s">
-        <v>127</v>
-      </c>
-      <c r="B141" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="C141" s="47" t="s">
+      <c r="C141" s="32" t="s">
         <v>26</v>
       </c>
       <c r="D141"/>
       <c r="E141" s="24" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="F141" s="24">
-        <v>696</v>
+        <v>328</v>
       </c>
       <c r="G141" s="24">
-        <v>1217</v>
+        <v>564</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A142" s="47" t="s">
-        <v>127</v>
-      </c>
-      <c r="B142" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="C142" s="47" t="s">
+      <c r="A142" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B142" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C142" s="32" t="s">
         <v>26</v>
       </c>
       <c r="D142"/>
       <c r="E142" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F142" s="24">
-        <v>1218</v>
+        <v>565</v>
       </c>
       <c r="G142" s="24">
-        <v>2483</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A143" s="47" t="s">
-        <v>127</v>
-      </c>
-      <c r="B143" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="C143" s="47" t="s">
+      <c r="A143" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B143" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C143" s="32" t="s">
         <v>26</v>
       </c>
       <c r="D143"/>
       <c r="E143" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="F143" s="24">
+        <v>1138</v>
+      </c>
+      <c r="G143" s="24">
+        <v>2199</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A144" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B144" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C144" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D144"/>
+      <c r="E144" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F144" s="24">
+        <v>2200</v>
+      </c>
+      <c r="G144" s="24">
+        <v>2910</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A145" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B145" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C145" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D145"/>
+      <c r="E145" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F145" s="24">
+        <v>2911</v>
+      </c>
+      <c r="G145" s="24">
+        <v>9498</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A146" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B146" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C146" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D146"/>
+      <c r="E146" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F146" s="24">
+        <v>2911</v>
+      </c>
+      <c r="G146" s="24">
+        <v>3630</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A147" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B147" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C147" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D147"/>
+      <c r="E147" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F147" s="24">
+        <v>3631</v>
+      </c>
+      <c r="G147" s="24">
+        <v>5514</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A148" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B148" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C148" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D148"/>
+      <c r="E148" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="F148" s="24">
+        <v>5515</v>
+      </c>
+      <c r="G148" s="24">
+        <v>5637</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A149" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B149" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C149" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D149"/>
+      <c r="E149" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="F149" s="24">
+        <v>5638</v>
+      </c>
+      <c r="G149" s="24">
+        <v>6423</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A150" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B150" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C150" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D150"/>
+      <c r="E150" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F150" s="24">
+        <v>6424</v>
+      </c>
+      <c r="G150" s="24">
+        <v>9498</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A151" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B151" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C151" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D151"/>
+      <c r="E151" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F151" s="24">
+        <v>6424</v>
+      </c>
+      <c r="G151" s="24">
+        <v>7797</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A152" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B152" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C152" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D152"/>
+      <c r="E152" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F143" s="24">
+      <c r="F152" s="24">
+        <v>7798</v>
+      </c>
+      <c r="G152" s="24">
+        <v>9498</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A153" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B153" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C153" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D153"/>
+      <c r="E153" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F153" s="24">
+        <v>9502</v>
+      </c>
+      <c r="G153" s="24">
+        <v>9867</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A154" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="B154" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C154" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D154"/>
+      <c r="E154" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F154" s="24">
+        <v>1</v>
+      </c>
+      <c r="G154" s="24">
+        <v>10479</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A155" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="B155" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C155" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D155"/>
+      <c r="E155" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F155" s="24">
+        <v>618</v>
+      </c>
+      <c r="G155" s="24">
+        <v>10187</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A156" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="B156" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C156" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D156"/>
+      <c r="E156" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="F156" s="24">
+        <v>618</v>
+      </c>
+      <c r="G156" s="24">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A157" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="B157" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C157" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D157"/>
+      <c r="E157" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="F157" s="24">
+        <v>696</v>
+      </c>
+      <c r="G157" s="24">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A158" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="B158" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C158" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D158"/>
+      <c r="E158" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="F158" s="24">
+        <v>1218</v>
+      </c>
+      <c r="G158" s="24">
+        <v>2483</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A159" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="B159" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C159" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D159"/>
+      <c r="E159" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F159" s="24">
         <v>8388</v>
       </c>
-      <c r="G143" s="24">
+      <c r="G159" s="24">
         <v>10184</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
         <v>52</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B160" t="s">
         <v>61</v>
       </c>
-      <c r="C144" s="16" t="s">
+      <c r="C160" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D144" s="20" t="s">
+      <c r="D160" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E160" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F160" s="24">
+        <v>1</v>
+      </c>
+      <c r="G160" s="24">
+        <v>19199</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>52</v>
+      </c>
+      <c r="B161" t="s">
+        <v>61</v>
+      </c>
+      <c r="C161" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D161" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E161" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F161" s="24">
+        <v>1</v>
+      </c>
+      <c r="G161" s="24">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>52</v>
+      </c>
+      <c r="B162" t="s">
+        <v>61</v>
+      </c>
+      <c r="C162" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D162" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E162" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F162" s="24">
+        <v>351</v>
+      </c>
+      <c r="G162" s="24">
+        <v>18068</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>52</v>
+      </c>
+      <c r="B163" t="s">
+        <v>61</v>
+      </c>
+      <c r="C163" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D163" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E163" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F163" s="24">
+        <v>18069</v>
+      </c>
+      <c r="G163" s="24">
+        <v>19199</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A164" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B164" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C164" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D164" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="E144" s="24" t="s">
+      <c r="E164" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="F144" s="24">
+      <c r="F164" s="24">
         <v>1</v>
       </c>
-      <c r="G144" s="24">
-        <v>19199</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
-        <v>52</v>
-      </c>
-      <c r="B145" t="s">
-        <v>61</v>
-      </c>
-      <c r="C145" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D145" s="20" t="s">
+      <c r="G164" s="24">
+        <v>18554</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A165" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B165" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C165" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D165" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="E145" s="24" t="s">
+      <c r="E165" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F145" s="24">
+      <c r="F165" s="24">
         <v>1</v>
       </c>
-      <c r="G145" s="24">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
-        <v>52</v>
-      </c>
-      <c r="B146" t="s">
-        <v>61</v>
-      </c>
-      <c r="C146" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D146" s="20" t="s">
+      <c r="G165" s="24">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A166" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B166" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C166" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D166" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="E146" s="24" t="s">
+      <c r="E166" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="F146" s="24">
-        <v>351</v>
-      </c>
-      <c r="G146" s="24">
-        <v>18068</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
-        <v>52</v>
-      </c>
-      <c r="B147" t="s">
-        <v>61</v>
-      </c>
-      <c r="C147" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D147" s="20" t="s">
+      <c r="F166" s="24">
+        <v>200</v>
+      </c>
+      <c r="G166" s="24">
+        <v>17905</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A167" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B167" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C167" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D167" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="E147" s="24" t="s">
+      <c r="E167" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F147" s="24">
-        <v>18069</v>
-      </c>
-      <c r="G147" s="24">
-        <v>19199</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A148" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="B148" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="C148" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="D148" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="E148" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="F148" s="24">
-        <v>1</v>
-      </c>
-      <c r="G148" s="24">
+      <c r="F167" s="24">
+        <v>17906</v>
+      </c>
+      <c r="G167" s="24">
         <v>18554</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A149" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="B149" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="C149" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="D149" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="E149" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="F149" s="24">
-        <v>1</v>
-      </c>
-      <c r="G149" s="24">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A150" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="B150" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="C150" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="D150" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="E150" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="F150" s="24">
-        <v>200</v>
-      </c>
-      <c r="G150" s="24">
-        <v>17905</v>
-      </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A151" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="B151" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="C151" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="D151" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="E151" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F151" s="24">
-        <v>17906</v>
-      </c>
-      <c r="G151" s="24">
-        <v>18554</v>
-      </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A152" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B152" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C152" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D152" s="24"/>
-      <c r="E152" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="F152" s="24">
-        <v>1</v>
-      </c>
-      <c r="G152" s="24">
-        <v>12573</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A153" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B153" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C153" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D153" s="24"/>
-      <c r="E153" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="F153" s="24">
-        <v>1</v>
-      </c>
-      <c r="G153" s="24">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A154" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B154" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C154" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D154" s="24"/>
-      <c r="E154" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="F154" s="24">
-        <v>386</v>
-      </c>
-      <c r="G154" s="24">
-        <v>12352</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A155" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B155" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C155" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D155" s="24"/>
-      <c r="E155" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="F155" s="24">
-        <v>386</v>
-      </c>
-      <c r="G155" s="24">
-        <v>3583</v>
-      </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A156" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B156" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C156" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D156" s="24"/>
-      <c r="E156" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="F156" s="24">
-        <v>386</v>
-      </c>
-      <c r="G156" s="24">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A157" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B157" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C157" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D157" s="24"/>
-      <c r="E157" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="F157" s="24">
-        <v>890</v>
-      </c>
-      <c r="G157" s="24">
-        <v>1195</v>
-      </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A158" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B158" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C158" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D158" s="24"/>
-      <c r="E158" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="F158" s="24">
-        <v>1196</v>
-      </c>
-      <c r="G158" s="24">
-        <v>1876</v>
-      </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A159" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B159" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C159" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D159" s="24"/>
-      <c r="E159" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F159" s="24">
-        <v>1877</v>
-      </c>
-      <c r="G159" s="24">
-        <v>2461</v>
-      </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A160" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B160" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C160" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D160" s="24"/>
-      <c r="E160" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="F160" s="24">
-        <v>2462</v>
-      </c>
-      <c r="G160" s="24">
-        <v>3583</v>
-      </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A161" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B161" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C161" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D161" s="24"/>
-      <c r="E161" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="F161" s="24">
-        <v>3584</v>
-      </c>
-      <c r="G161" s="24">
-        <v>3793</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A162" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B162" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C162" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D162" s="24"/>
-      <c r="E162" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F162" s="24">
-        <v>3794</v>
-      </c>
-      <c r="G162" s="24">
-        <v>7471</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A163" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B163" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C163" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D163" s="24"/>
-      <c r="E163" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="F163" s="24">
-        <v>7472</v>
-      </c>
-      <c r="G163" s="24">
-        <v>7663</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A164" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B164" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C164" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D164" s="24"/>
-      <c r="E164" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="F164" s="24">
-        <v>7664</v>
-      </c>
-      <c r="G164" s="24">
-        <v>8704</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A165" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B165" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C165" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D165" s="24"/>
-      <c r="E165" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F165" s="24">
-        <v>8705</v>
-      </c>
-      <c r="G165" s="24">
-        <v>12349</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A166" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B166" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C166" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D166" s="24"/>
-      <c r="E166" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="F166" s="24">
-        <v>8705</v>
-      </c>
-      <c r="G166" s="24">
-        <v>10192</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A167" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B167" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C167" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D167" s="24"/>
-      <c r="E167" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="F167" s="24">
-        <v>10193</v>
-      </c>
-      <c r="G167" s="24">
-        <v>12349</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.2">
@@ -9799,620 +9948,1018 @@
         <v>35</v>
       </c>
       <c r="B168" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C168" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D168" s="24"/>
+      <c r="D168" s="24" t="s">
+        <v>157</v>
+      </c>
       <c r="E168" s="24" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="F168" s="24">
-        <v>12360</v>
+        <v>1</v>
       </c>
       <c r="G168" s="24">
         <v>12573</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A169" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B169" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C169" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D169" s="24"/>
+      <c r="A169" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B169" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C169" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D169" s="24" t="s">
+        <v>157</v>
+      </c>
       <c r="E169" s="24" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="F169" s="24">
         <v>1</v>
       </c>
       <c r="G169" s="24">
-        <v>10053</v>
+        <v>385</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A170" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B170" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C170" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D170" s="24"/>
+      <c r="A170" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B170" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C170" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D170" s="24" t="s">
+        <v>157</v>
+      </c>
       <c r="E170" s="24" t="s">
         <v>66</v>
       </c>
       <c r="F170" s="24">
-        <v>1</v>
+        <v>386</v>
       </c>
       <c r="G170" s="24">
-        <v>10053</v>
+        <v>12352</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A171" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B171" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C171" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D171" s="24"/>
+      <c r="A171" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B171" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C171" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D171" s="24" t="s">
+        <v>157</v>
+      </c>
       <c r="E171" s="24" t="s">
         <v>101</v>
       </c>
       <c r="F171" s="24">
+        <v>386</v>
+      </c>
+      <c r="G171" s="24">
+        <v>3583</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A172" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B172" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C172" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D172" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E172" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="F172" s="24">
+        <v>386</v>
+      </c>
+      <c r="G172" s="24">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A173" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B173" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C173" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D173" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E173" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F173" s="24">
+        <v>890</v>
+      </c>
+      <c r="G173" s="24">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A174" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B174" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C174" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D174" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E174" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F174" s="24">
+        <v>1196</v>
+      </c>
+      <c r="G174" s="24">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A175" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B175" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C175" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D175" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E175" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F175" s="24">
+        <v>1877</v>
+      </c>
+      <c r="G175" s="24">
+        <v>2461</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A176" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B176" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C176" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D176" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E176" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="F176" s="24">
+        <v>2462</v>
+      </c>
+      <c r="G176" s="24">
+        <v>3583</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A177" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B177" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C177" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D177" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E177" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="F177" s="24">
+        <v>3584</v>
+      </c>
+      <c r="G177" s="24">
+        <v>3793</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A178" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B178" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C178" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D178" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E178" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F178" s="24">
+        <v>3794</v>
+      </c>
+      <c r="G178" s="24">
+        <v>7471</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A179" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B179" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C179" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D179" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E179" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="F179" s="24">
+        <v>7472</v>
+      </c>
+      <c r="G179" s="24">
+        <v>7663</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A180" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B180" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C180" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D180" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E180" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="F180" s="24">
+        <v>7664</v>
+      </c>
+      <c r="G180" s="24">
+        <v>8704</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A181" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B181" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C181" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D181" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E181" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F181" s="24">
+        <v>8705</v>
+      </c>
+      <c r="G181" s="24">
+        <v>12349</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A182" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B182" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C182" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D182" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E182" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F182" s="24">
+        <v>8705</v>
+      </c>
+      <c r="G182" s="24">
+        <v>10192</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A183" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B183" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C183" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D183" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E183" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F183" s="24">
+        <v>10193</v>
+      </c>
+      <c r="G183" s="24">
+        <v>12349</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A184" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B184" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C184" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D184" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E184" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F184" s="24">
+        <v>12360</v>
+      </c>
+      <c r="G184" s="24">
+        <v>12573</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A185" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="B185" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="C185" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D185" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="E185" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F185" s="24">
         <v>1</v>
       </c>
-      <c r="G171" s="24">
-        <v>2358</v>
-      </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A172" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B172" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C172" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D172" s="24"/>
-      <c r="E172" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="F172" s="24">
+      <c r="G185" s="24">
+        <v>12983</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A186" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="B186" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="C186" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D186" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="E186" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F186" s="24">
+        <v>499</v>
+      </c>
+      <c r="G186" s="24">
+        <v>12480</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A187" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="B187" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="C187" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D187" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="E187" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F187" s="24">
         <v>1</v>
       </c>
-      <c r="G172" s="24">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A173" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B173" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C173" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D173" s="24"/>
-      <c r="E173" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="F173" s="24">
-        <v>346</v>
-      </c>
-      <c r="G173" s="24">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A174" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B174" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C174" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D174" s="24"/>
-      <c r="E174" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="F174" s="24">
-        <v>655</v>
-      </c>
-      <c r="G174" s="24">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A175" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B175" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C175" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D175" s="24"/>
-      <c r="E175" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F175" s="24">
-        <v>853</v>
-      </c>
-      <c r="G175" s="24">
-        <v>2358</v>
-      </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A176" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B176" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C176" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D176" s="24"/>
-      <c r="E176" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="F176" s="24">
-        <v>2359</v>
-      </c>
-      <c r="G176" s="24">
-        <v>10050</v>
-      </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A177" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B177" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C177" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D177" s="24"/>
-      <c r="E177" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F177" s="24">
-        <v>2359</v>
-      </c>
-      <c r="G177" s="24">
-        <v>3390</v>
-      </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A178" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B178" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C178" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D178" s="24"/>
-      <c r="E178" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F178" s="24">
-        <v>3391</v>
-      </c>
-      <c r="G178" s="24">
-        <v>3978</v>
-      </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A179" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B179" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C179" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D179" s="24"/>
-      <c r="E179" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="F179" s="24">
-        <v>3979</v>
-      </c>
-      <c r="G179" s="24">
-        <v>4431</v>
-      </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A180" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B180" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C180" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D180" s="24"/>
-      <c r="E180" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F180" s="24">
-        <v>4432</v>
-      </c>
-      <c r="G180" s="24">
-        <v>6303</v>
-      </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A181" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B181" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C181" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D181" s="24"/>
-      <c r="E181" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F181" s="24">
-        <v>6304</v>
-      </c>
-      <c r="G181" s="24">
-        <v>6687</v>
-      </c>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A182" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B182" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C182" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D182" s="24"/>
-      <c r="E182" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="F182" s="24">
-        <v>6688</v>
-      </c>
-      <c r="G182" s="24">
-        <v>6762</v>
-      </c>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A183" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B183" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C183" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D183" s="24"/>
-      <c r="E183" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="F183" s="24">
-        <v>6763</v>
-      </c>
-      <c r="G183" s="24">
-        <v>7557</v>
-      </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A184" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B184" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C184" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D184" s="24"/>
-      <c r="E184" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F184" s="24">
-        <v>7558</v>
-      </c>
-      <c r="G184" s="24">
-        <v>10050</v>
-      </c>
-      <c r="H184" s="22"/>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A185" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="B185" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="C185" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="D185" s="24"/>
-      <c r="E185" t="s">
+      <c r="G187" s="24">
+        <v>11276</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A188" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="B188" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="C188" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D188" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="E188" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F188" s="24">
+        <v>124</v>
+      </c>
+      <c r="G188" s="24">
+        <v>11031</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A189" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="B189" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="C189" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D189" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="E189" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="F185">
+      <c r="F189" s="24">
         <v>1</v>
       </c>
-      <c r="G185">
-        <v>5938</v>
-      </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A186" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="B186" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="C186" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="D186" s="24"/>
-      <c r="E186" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="F186" s="24">
-        <v>117</v>
-      </c>
-      <c r="G186" s="24">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A187" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="B187" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="C187" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="D187" s="24"/>
-      <c r="E187" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="F187">
-        <f t="shared" ref="F187" si="0">(D187+2824)</f>
-        <v>2824</v>
-      </c>
-      <c r="G187" s="24">
-        <v>5673</v>
-      </c>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A188" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="B188" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="C188" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="D188" s="24"/>
-      <c r="E188" t="s">
-        <v>79</v>
-      </c>
-      <c r="F188" s="24">
-        <v>1</v>
-      </c>
-      <c r="G188" s="24">
-        <v>3114</v>
-      </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A189" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="B189" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="C189" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="D189" s="24"/>
-      <c r="E189" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="F189">
-        <v>105</v>
-      </c>
-      <c r="G189">
-        <v>2849</v>
-      </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A190" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="B190" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="C190" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="D190" s="24"/>
-      <c r="E190" t="s">
-        <v>79</v>
+      <c r="G189" s="24">
+        <v>7797</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A190" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="B190" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="C190" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D190" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="E190" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="F190" s="24">
         <v>1</v>
       </c>
       <c r="G190" s="24">
-        <v>2824</v>
-      </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7770</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" s="24" t="s">
-        <v>119</v>
+        <v>50</v>
       </c>
       <c r="B191" s="24" t="s">
-        <v>119</v>
+        <v>59</v>
       </c>
       <c r="C191" s="24" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="D191" s="24"/>
       <c r="E191" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="F191">
+        <v>79</v>
+      </c>
+      <c r="F191" s="24">
+        <v>1</v>
+      </c>
+      <c r="G191" s="24">
+        <v>10053</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A192" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B192" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C192" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D192" s="24"/>
+      <c r="E192" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F192" s="24">
+        <v>1</v>
+      </c>
+      <c r="G192" s="24">
+        <v>10053</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A193" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B193" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C193" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D193" s="24"/>
+      <c r="E193" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F193" s="24">
+        <v>1</v>
+      </c>
+      <c r="G193" s="24">
+        <v>2358</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A194" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B194" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C194" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D194" s="24"/>
+      <c r="E194" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="F194" s="24">
+        <v>1</v>
+      </c>
+      <c r="G194" s="24">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A195" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B195" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C195" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D195" s="24"/>
+      <c r="E195" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F195" s="24">
+        <v>346</v>
+      </c>
+      <c r="G195" s="24">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A196" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B196" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C196" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D196" s="24"/>
+      <c r="E196" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="F196" s="24">
+        <v>655</v>
+      </c>
+      <c r="G196" s="24">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A197" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B197" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C197" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D197" s="24"/>
+      <c r="E197" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="F197" s="24">
+        <v>853</v>
+      </c>
+      <c r="G197" s="24">
+        <v>2358</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A198" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B198" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C198" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D198" s="24"/>
+      <c r="E198" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F198" s="24">
+        <v>2359</v>
+      </c>
+      <c r="G198" s="24">
+        <v>10050</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A199" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B199" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C199" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D199" s="24"/>
+      <c r="E199" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F199" s="24">
+        <v>2359</v>
+      </c>
+      <c r="G199" s="24">
+        <v>3390</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A200" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B200" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C200" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D200" s="24"/>
+      <c r="E200" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F200" s="24">
+        <v>3391</v>
+      </c>
+      <c r="G200" s="24">
+        <v>3978</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A201" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B201" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C201" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D201" s="24"/>
+      <c r="E201" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="F201" s="24">
+        <v>3979</v>
+      </c>
+      <c r="G201" s="24">
+        <v>4431</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A202" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B202" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C202" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D202" s="24"/>
+      <c r="E202" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F202" s="24">
+        <v>4432</v>
+      </c>
+      <c r="G202" s="24">
+        <v>6303</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A203" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B203" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C203" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D203" s="24"/>
+      <c r="E203" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F203" s="24">
+        <v>6304</v>
+      </c>
+      <c r="G203" s="24">
+        <v>6687</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A204" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B204" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C204" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D204" s="24"/>
+      <c r="E204" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F204" s="24">
+        <v>6688</v>
+      </c>
+      <c r="G204" s="24">
+        <v>6762</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A205" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B205" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C205" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D205" s="24"/>
+      <c r="E205" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="F205" s="24">
+        <v>6763</v>
+      </c>
+      <c r="G205" s="24">
+        <v>7557</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A206" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B206" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C206" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D206" s="24"/>
+      <c r="E206" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F206" s="24">
+        <v>7558</v>
+      </c>
+      <c r="G206" s="24">
+        <v>10050</v>
+      </c>
+      <c r="H206" s="22"/>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A207" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="B207" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C207" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D207" s="24"/>
+      <c r="E207" t="s">
+        <v>79</v>
+      </c>
+      <c r="F207">
+        <v>1</v>
+      </c>
+      <c r="G207">
+        <v>5938</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A208" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="B208" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C208" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D208" s="24"/>
+      <c r="E208" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="F208" s="24">
         <v>117</v>
       </c>
-      <c r="G191">
+      <c r="G208" s="24">
         <v>2543</v>
       </c>
     </row>
-    <row r="226" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B226" s="1"/>
-      <c r="C226" s="5"/>
-    </row>
-    <row r="227" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B227" s="1"/>
-      <c r="C227" s="5"/>
-      <c r="D227" s="5"/>
-    </row>
-    <row r="228" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B228" s="1"/>
-      <c r="C228" s="5"/>
-      <c r="D228" s="5"/>
-    </row>
-    <row r="229" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B229" s="1"/>
-      <c r="C229" s="5"/>
-      <c r="D229" s="5"/>
-    </row>
-    <row r="230" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B230" s="1"/>
-      <c r="C230" s="5"/>
-      <c r="D230" s="5"/>
-    </row>
-    <row r="231" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B231" s="1"/>
-      <c r="C231" s="5"/>
-      <c r="D231" s="5"/>
-    </row>
-    <row r="232" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B232" s="1"/>
-      <c r="C232" s="5"/>
-      <c r="D232" s="5"/>
-    </row>
-    <row r="233" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B233" s="1"/>
-      <c r="C233" s="5"/>
-      <c r="D233" s="5"/>
-    </row>
-    <row r="234" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B234" s="1"/>
-      <c r="C234" s="5"/>
-      <c r="D234" s="5"/>
-    </row>
-    <row r="235" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B235" s="1"/>
-      <c r="C235" s="5"/>
-      <c r="D235" s="5"/>
-    </row>
-    <row r="236" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B236" s="1"/>
-      <c r="C236" s="5"/>
-      <c r="D236" s="5"/>
-    </row>
-    <row r="237" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B237" s="1"/>
-      <c r="C237" s="5"/>
-      <c r="D237" s="5"/>
-    </row>
-    <row r="238" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B238" s="1"/>
-      <c r="C238" s="5"/>
-      <c r="D238" s="5"/>
-    </row>
-    <row r="239" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B239" s="1"/>
-      <c r="C239" s="5"/>
-      <c r="D239" s="5"/>
-    </row>
-    <row r="240" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B240" s="1"/>
-      <c r="C240" s="5"/>
-      <c r="D240" s="5"/>
-    </row>
-    <row r="241" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B241" s="1"/>
-      <c r="C241" s="5"/>
-      <c r="D241" s="5"/>
-    </row>
-    <row r="242" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B242" s="1"/>
-      <c r="C242" s="5"/>
-      <c r="D242" s="5"/>
-    </row>
-    <row r="243" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B243" s="1"/>
-      <c r="C243" s="5"/>
-      <c r="D243" s="5"/>
-    </row>
-    <row r="244" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B244" s="1"/>
-      <c r="C244" s="5"/>
-      <c r="D244" s="5"/>
-    </row>
-    <row r="245" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B245" s="1"/>
-      <c r="C245" s="5"/>
-      <c r="D245" s="5"/>
-    </row>
-    <row r="246" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B246" s="1"/>
-      <c r="C246" s="5"/>
-      <c r="D246" s="5"/>
-    </row>
-    <row r="247" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B247" s="1"/>
-      <c r="C247" s="5"/>
-      <c r="D247" s="5"/>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A209" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="B209" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C209" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D209" s="24"/>
+      <c r="E209" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="F209">
+        <f t="shared" ref="F209" si="0">(D209+2824)</f>
+        <v>2824</v>
+      </c>
+      <c r="G209" s="24">
+        <v>5673</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A210" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B210" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C210" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D210" s="24"/>
+      <c r="E210" t="s">
+        <v>79</v>
+      </c>
+      <c r="F210" s="24">
+        <v>1</v>
+      </c>
+      <c r="G210" s="24">
+        <v>3114</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A211" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B211" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C211" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D211" s="24"/>
+      <c r="E211" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="F211">
+        <v>105</v>
+      </c>
+      <c r="G211">
+        <v>2849</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A212" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B212" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C212" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D212" s="24"/>
+      <c r="E212" t="s">
+        <v>79</v>
+      </c>
+      <c r="F212" s="24">
+        <v>1</v>
+      </c>
+      <c r="G212" s="24">
+        <v>2824</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A213" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B213" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C213" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D213" s="24"/>
+      <c r="E213" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="F213">
+        <v>117</v>
+      </c>
+      <c r="G213">
+        <v>2543</v>
+      </c>
     </row>
     <row r="248" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B248" s="1"/>
       <c r="C248" s="5"/>
-      <c r="D248" s="5"/>
     </row>
     <row r="249" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B249" s="1"/>
@@ -10421,11 +10968,13 @@
     </row>
     <row r="250" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B250" s="1"/>
+      <c r="C250" s="5"/>
       <c r="D250" s="5"/>
     </row>
     <row r="251" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B251" s="1"/>
       <c r="C251" s="5"/>
+      <c r="D251" s="5"/>
     </row>
     <row r="252" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B252" s="1"/>
@@ -10458,66 +11007,180 @@
       <c r="D257" s="5"/>
     </row>
     <row r="258" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B258" s="1"/>
+      <c r="C258" s="5"/>
       <c r="D258" s="5"/>
     </row>
-    <row r="940" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E940" s="1"/>
-    </row>
-    <row r="1076" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1076" s="1"/>
-    </row>
-    <row r="1077" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1077" s="1"/>
-    </row>
-    <row r="1202" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1202" s="1"/>
-    </row>
-    <row r="1203" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1203" s="1"/>
-    </row>
-    <row r="1204" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1204" s="1"/>
-    </row>
-    <row r="1205" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1205" s="1"/>
-    </row>
-    <row r="1206" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1206" s="1"/>
-    </row>
-    <row r="1207" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1207" s="1"/>
-    </row>
-    <row r="1252" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E1252" s="1"/>
-      <c r="F1252" s="1"/>
-    </row>
-    <row r="1253" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E1253" s="1"/>
-      <c r="F1253" s="1"/>
-    </row>
-    <row r="1254" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E1254" s="1"/>
-      <c r="F1254" s="1"/>
-    </row>
-    <row r="1256" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1256" s="1"/>
-    </row>
-    <row r="1257" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1257" s="1"/>
-    </row>
-    <row r="1258" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1258" s="1"/>
-    </row>
-    <row r="1259" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1259" s="1"/>
-    </row>
-    <row r="1260" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1260" s="1"/>
-    </row>
-    <row r="1279" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="259" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B259" s="1"/>
+      <c r="C259" s="5"/>
+      <c r="D259" s="5"/>
+    </row>
+    <row r="260" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B260" s="1"/>
+      <c r="C260" s="5"/>
+      <c r="D260" s="5"/>
+    </row>
+    <row r="261" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B261" s="1"/>
+      <c r="C261" s="5"/>
+      <c r="D261" s="5"/>
+    </row>
+    <row r="262" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B262" s="1"/>
+      <c r="C262" s="5"/>
+      <c r="D262" s="5"/>
+    </row>
+    <row r="263" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B263" s="1"/>
+      <c r="C263" s="5"/>
+      <c r="D263" s="5"/>
+    </row>
+    <row r="264" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B264" s="1"/>
+      <c r="C264" s="5"/>
+      <c r="D264" s="5"/>
+    </row>
+    <row r="265" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B265" s="1"/>
+      <c r="C265" s="5"/>
+      <c r="D265" s="5"/>
+    </row>
+    <row r="266" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B266" s="1"/>
+      <c r="C266" s="5"/>
+      <c r="D266" s="5"/>
+    </row>
+    <row r="267" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B267" s="1"/>
+      <c r="C267" s="5"/>
+      <c r="D267" s="5"/>
+    </row>
+    <row r="268" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B268" s="1"/>
+      <c r="C268" s="5"/>
+      <c r="D268" s="5"/>
+    </row>
+    <row r="269" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B269" s="1"/>
+      <c r="C269" s="5"/>
+      <c r="D269" s="5"/>
+    </row>
+    <row r="270" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B270" s="1"/>
+      <c r="C270" s="5"/>
+      <c r="D270" s="5"/>
+    </row>
+    <row r="271" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B271" s="1"/>
+      <c r="C271" s="5"/>
+      <c r="D271" s="5"/>
+    </row>
+    <row r="272" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B272" s="1"/>
+      <c r="D272" s="5"/>
+    </row>
+    <row r="273" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B273" s="1"/>
+      <c r="C273" s="5"/>
+    </row>
+    <row r="274" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B274" s="1"/>
+      <c r="C274" s="5"/>
+      <c r="D274" s="5"/>
+    </row>
+    <row r="275" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B275" s="1"/>
+      <c r="C275" s="5"/>
+      <c r="D275" s="5"/>
+    </row>
+    <row r="276" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B276" s="1"/>
+      <c r="C276" s="5"/>
+      <c r="D276" s="5"/>
+    </row>
+    <row r="277" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B277" s="1"/>
+      <c r="C277" s="5"/>
+      <c r="D277" s="5"/>
+    </row>
+    <row r="278" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B278" s="1"/>
+      <c r="C278" s="5"/>
+      <c r="D278" s="5"/>
+    </row>
+    <row r="279" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B279" s="1"/>
+      <c r="C279" s="5"/>
+      <c r="D279" s="5"/>
+    </row>
+    <row r="280" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D280" s="5"/>
+    </row>
+    <row r="962" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C962"/>
+      <c r="D962"/>
+      <c r="E962" s="1"/>
+    </row>
+    <row r="1098" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1098" s="1"/>
+      <c r="C1098"/>
+      <c r="D1098"/>
+    </row>
+    <row r="1099" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1099" s="1"/>
+      <c r="C1099"/>
+      <c r="D1099"/>
+    </row>
+    <row r="1224" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1224" s="1"/>
+      <c r="C1224"/>
+      <c r="D1224"/>
+    </row>
+    <row r="1225" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1225" s="1"/>
+      <c r="C1225"/>
+      <c r="D1225"/>
+    </row>
+    <row r="1226" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1226" s="1"/>
+      <c r="C1226"/>
+      <c r="D1226"/>
+    </row>
+    <row r="1227" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1227" s="1"/>
+      <c r="C1227"/>
+      <c r="D1227"/>
+    </row>
+    <row r="1228" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1228" s="1"/>
+      <c r="C1228"/>
+      <c r="D1228"/>
+    </row>
+    <row r="1229" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1229" s="1"/>
+      <c r="C1229"/>
+      <c r="D1229"/>
+    </row>
+    <row r="1274" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E1274" s="1"/>
+      <c r="F1274" s="1"/>
+    </row>
+    <row r="1275" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E1275" s="1"/>
+      <c r="F1275" s="1"/>
+    </row>
+    <row r="1276" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E1276" s="1"/>
+      <c r="F1276" s="1"/>
+    </row>
+    <row r="1278" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1278" s="1"/>
+    </row>
+    <row r="1279" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1279" s="1"/>
     </row>
-    <row r="1280" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1280" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1280" s="1"/>
     </row>
     <row r="1281" spans="2:2" x14ac:dyDescent="0.2">
@@ -10526,117 +11189,191 @@
     <row r="1282" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1282" s="1"/>
     </row>
-    <row r="1283" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1283" s="1"/>
-    </row>
-    <row r="1284" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1284" s="1"/>
-    </row>
-    <row r="1285" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1285" s="1"/>
-    </row>
-    <row r="1287" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1287" s="1"/>
-    </row>
-    <row r="1288" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1288" s="1"/>
-    </row>
-    <row r="1289" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1289" s="1"/>
-    </row>
-    <row r="1290" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1290" s="1"/>
-    </row>
-    <row r="1291" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1291" s="1"/>
-    </row>
-    <row r="1292" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1292" s="1"/>
-    </row>
-    <row r="1344" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1344" s="1"/>
-    </row>
-    <row r="1345" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1345" s="1"/>
-    </row>
-    <row r="1346" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1346" s="1"/>
-    </row>
-    <row r="1347" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1347" s="1"/>
-    </row>
-    <row r="1349" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1349" s="1"/>
-    </row>
-    <row r="1350" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1350" s="1"/>
-    </row>
-    <row r="1351" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1351" s="1"/>
-    </row>
-    <row r="1352" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1352" s="1"/>
-    </row>
-    <row r="1387" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1387" s="1"/>
-    </row>
-    <row r="1388" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1388" s="1"/>
-    </row>
-    <row r="1389" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1389" s="1"/>
-    </row>
-    <row r="1390" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1390" s="1"/>
-    </row>
-    <row r="1391" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1391" s="1"/>
-    </row>
-    <row r="1392" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1392" s="1"/>
-    </row>
-    <row r="1434" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E1434" s="1"/>
-      <c r="F1434" s="1"/>
-    </row>
-    <row r="1435" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C1435" s="6"/>
-      <c r="E1435" s="1"/>
-      <c r="F1435" s="1"/>
-    </row>
-    <row r="1436" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C1436" s="6"/>
-      <c r="D1436" s="6"/>
-      <c r="E1436" s="1"/>
-      <c r="F1436" s="1"/>
-    </row>
-    <row r="1437" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C1437" s="6"/>
-      <c r="D1437" s="6"/>
-      <c r="E1437" s="1"/>
-      <c r="F1437" s="1"/>
-    </row>
-    <row r="1438" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D1438" s="6"/>
-      <c r="E1438" s="1"/>
-      <c r="F1438" s="1"/>
-    </row>
-    <row r="1501" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1501" s="1"/>
-    </row>
-    <row r="1502" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1502" s="1"/>
-    </row>
-    <row r="1503" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1503" s="1"/>
-    </row>
-    <row r="1504" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1504" s="1"/>
+    <row r="1301" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1301" s="1"/>
+      <c r="C1301"/>
+      <c r="D1301"/>
+    </row>
+    <row r="1302" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1302" s="1"/>
+      <c r="C1302"/>
+      <c r="D1302"/>
+    </row>
+    <row r="1303" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1303" s="1"/>
+      <c r="C1303"/>
+      <c r="D1303"/>
+    </row>
+    <row r="1304" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1304" s="1"/>
+      <c r="C1304"/>
+      <c r="D1304"/>
+    </row>
+    <row r="1305" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1305" s="1"/>
+      <c r="C1305"/>
+      <c r="D1305"/>
+    </row>
+    <row r="1306" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1306" s="1"/>
+      <c r="C1306"/>
+      <c r="D1306"/>
+    </row>
+    <row r="1307" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1307" s="1"/>
+      <c r="C1307"/>
+      <c r="D1307"/>
+    </row>
+    <row r="1309" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1309" s="1"/>
+      <c r="C1309"/>
+      <c r="D1309"/>
+    </row>
+    <row r="1310" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1310" s="1"/>
+      <c r="C1310"/>
+      <c r="D1310"/>
+    </row>
+    <row r="1311" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1311" s="1"/>
+      <c r="C1311"/>
+      <c r="D1311"/>
+    </row>
+    <row r="1312" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1312" s="1"/>
+      <c r="C1312"/>
+      <c r="D1312"/>
+    </row>
+    <row r="1313" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1313" s="1"/>
+      <c r="C1313"/>
+      <c r="D1313"/>
+    </row>
+    <row r="1314" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1314" s="1"/>
+      <c r="C1314"/>
+      <c r="D1314"/>
+    </row>
+    <row r="1366" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1366" s="1"/>
+      <c r="C1366"/>
+      <c r="D1366"/>
+    </row>
+    <row r="1367" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1367" s="1"/>
+      <c r="C1367"/>
+      <c r="D1367"/>
+    </row>
+    <row r="1368" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1368" s="1"/>
+      <c r="C1368"/>
+      <c r="D1368"/>
+    </row>
+    <row r="1369" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1369" s="1"/>
+      <c r="C1369"/>
+      <c r="D1369"/>
+    </row>
+    <row r="1371" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1371" s="1"/>
+      <c r="C1371"/>
+      <c r="D1371"/>
+    </row>
+    <row r="1372" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1372" s="1"/>
+      <c r="C1372"/>
+      <c r="D1372"/>
+    </row>
+    <row r="1373" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1373" s="1"/>
+      <c r="C1373"/>
+      <c r="D1373"/>
+    </row>
+    <row r="1374" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1374" s="1"/>
+      <c r="C1374"/>
+      <c r="D1374"/>
+    </row>
+    <row r="1409" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1409" s="1"/>
+      <c r="C1409"/>
+      <c r="D1409"/>
+    </row>
+    <row r="1410" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1410" s="1"/>
+      <c r="C1410"/>
+      <c r="D1410"/>
+    </row>
+    <row r="1411" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1411" s="1"/>
+      <c r="C1411"/>
+      <c r="D1411"/>
+    </row>
+    <row r="1412" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1412" s="1"/>
+      <c r="C1412"/>
+      <c r="D1412"/>
+    </row>
+    <row r="1413" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1413" s="1"/>
+      <c r="C1413"/>
+      <c r="D1413"/>
+    </row>
+    <row r="1414" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1414" s="1"/>
+      <c r="C1414"/>
+      <c r="D1414"/>
+    </row>
+    <row r="1456" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E1456" s="1"/>
+      <c r="F1456" s="1"/>
+    </row>
+    <row r="1457" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C1457" s="6"/>
+      <c r="E1457" s="1"/>
+      <c r="F1457" s="1"/>
+    </row>
+    <row r="1458" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C1458" s="6"/>
+      <c r="D1458" s="6"/>
+      <c r="E1458" s="1"/>
+      <c r="F1458" s="1"/>
+    </row>
+    <row r="1459" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C1459" s="6"/>
+      <c r="D1459" s="6"/>
+      <c r="E1459" s="1"/>
+      <c r="F1459" s="1"/>
+    </row>
+    <row r="1460" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D1460" s="6"/>
+      <c r="E1460" s="1"/>
+      <c r="F1460" s="1"/>
+    </row>
+    <row r="1523" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1523" s="1"/>
+      <c r="C1523"/>
+      <c r="D1523"/>
+    </row>
+    <row r="1524" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1524" s="1"/>
+      <c r="C1524"/>
+      <c r="D1524"/>
+    </row>
+    <row r="1525" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1525" s="1"/>
+      <c r="C1525"/>
+      <c r="D1525"/>
+    </row>
+    <row r="1526" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1526" s="1"/>
+      <c r="C1526"/>
+      <c r="D1526"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G1457">
-    <sortCondition ref="C2:C1457"/>
-    <sortCondition ref="D2:D1457"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G1479">
+    <sortCondition ref="C2:C1479"/>
+    <sortCondition ref="D2:D1479"/>
   </sortState>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -10661,10 +11398,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="45" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C1" s="46" t="s">
         <v>14</v>
@@ -10684,10 +11421,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="45" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" s="46" t="s">
         <v>14</v>
@@ -10707,10 +11444,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" s="46" t="s">
         <v>14</v>
@@ -10730,10 +11467,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C4" s="46" t="s">
         <v>14</v>
@@ -10762,7 +11499,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E5" s="23" t="s">
         <v>79</v>
@@ -10785,7 +11522,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E6" s="23" t="s">
         <v>15</v>
@@ -10808,7 +11545,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E7" s="23" t="s">
         <v>66</v>
@@ -10831,7 +11568,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E8" s="23" t="s">
         <v>11</v>
@@ -10845,16 +11582,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C9" s="44" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>79</v>
@@ -10868,16 +11605,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B10" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C10" s="44" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>66</v>
@@ -10891,16 +11628,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B11" s="43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C11" s="44" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>79</v>
@@ -10914,16 +11651,16 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B12" s="43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C12" s="44" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>66</v>
@@ -12015,16 +12752,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E1" s="24" t="s">
         <v>10</v>
@@ -12046,16 +12783,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E2" s="24" t="s">
         <v>66</v>
@@ -12077,16 +12814,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
         <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E3" t="s">
         <v>79</v>
@@ -12108,19 +12845,19 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>110</v>
-      </c>
       <c r="C4" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F4" s="24">
         <v>117</v>
@@ -12131,16 +12868,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
         <v>109</v>
       </c>
-      <c r="B5" t="s">
-        <v>110</v>
-      </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
Dinucs and nucs broken down by feature
</commit_message>
<xml_diff>
--- a/tabular/core/flavi-reference_feature_locations.xlsx
+++ b/tabular/core/flavi-reference_feature_locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flavivirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EABFC2A-3A64-0A4B-B43F-6D79CB5014E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC5ECCE-EB99-5C42-B5F7-96F7EECD4A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9280" yWindow="500" windowWidth="28800" windowHeight="16620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="172">
   <si>
     <t>featureName</t>
   </si>
@@ -6148,10 +6148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1526"/>
+  <dimension ref="A1:H1525"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G183" sqref="G183"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A163" sqref="A163:XFD163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9843,7 +9843,7 @@
         <v>1</v>
       </c>
       <c r="G160" s="24">
-        <v>19199</v>
+        <v>10861</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
@@ -9889,34 +9889,34 @@
         <v>351</v>
       </c>
       <c r="G162" s="24">
-        <v>18068</v>
+        <v>10861</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
-        <v>52</v>
-      </c>
-      <c r="B163" t="s">
-        <v>161</v>
-      </c>
-      <c r="C163" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D163" s="20" t="s">
-        <v>97</v>
+      <c r="A163" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B163" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C163" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D163" s="24" t="s">
+        <v>98</v>
       </c>
       <c r="E163" s="24" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="F163" s="24">
-        <v>18069</v>
+        <v>1</v>
       </c>
       <c r="G163" s="24">
-        <v>19199</v>
+        <v>18554</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A164" s="29" t="s">
+      <c r="A164" s="31" t="s">
         <v>73</v>
       </c>
       <c r="B164" s="29" t="s">
@@ -9929,13 +9929,13 @@
         <v>98</v>
       </c>
       <c r="E164" s="24" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="F164" s="24">
         <v>1</v>
       </c>
       <c r="G164" s="24">
-        <v>18554</v>
+        <v>199</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
@@ -9952,13 +9952,13 @@
         <v>98</v>
       </c>
       <c r="E165" s="24" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="F165" s="24">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="G165" s="24">
-        <v>199</v>
+        <v>17905</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
@@ -9975,36 +9975,36 @@
         <v>98</v>
       </c>
       <c r="E166" s="24" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="F166" s="24">
-        <v>200</v>
+        <v>17906</v>
       </c>
       <c r="G166" s="24">
-        <v>17905</v>
+        <v>18554</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A167" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="B167" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="C167" s="30" t="s">
-        <v>74</v>
+      <c r="A167" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B167" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="C167" s="27" t="s">
+        <v>27</v>
       </c>
       <c r="D167" s="24" t="s">
-        <v>98</v>
+        <v>135</v>
       </c>
       <c r="E167" s="24" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="F167" s="24">
-        <v>17906</v>
+        <v>1</v>
       </c>
       <c r="G167" s="24">
-        <v>18554</v>
+        <v>12573</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.2">
@@ -10021,13 +10021,13 @@
         <v>135</v>
       </c>
       <c r="E168" s="24" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="F168" s="24">
         <v>1</v>
       </c>
       <c r="G168" s="24">
-        <v>12573</v>
+        <v>385</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.2">
@@ -10044,13 +10044,13 @@
         <v>135</v>
       </c>
       <c r="E169" s="24" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="F169" s="24">
-        <v>1</v>
+        <v>386</v>
       </c>
       <c r="G169" s="24">
-        <v>385</v>
+        <v>12352</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
@@ -10067,13 +10067,13 @@
         <v>135</v>
       </c>
       <c r="E170" s="24" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="F170" s="24">
         <v>386</v>
       </c>
       <c r="G170" s="24">
-        <v>12352</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.2">
@@ -10090,13 +10090,13 @@
         <v>135</v>
       </c>
       <c r="E171" s="24" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="F171" s="24">
         <v>386</v>
       </c>
       <c r="G171" s="24">
-        <v>3583</v>
+        <v>889</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.2">
@@ -10113,13 +10113,13 @@
         <v>135</v>
       </c>
       <c r="E172" s="24" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="F172" s="24">
-        <v>386</v>
+        <v>890</v>
       </c>
       <c r="G172" s="24">
-        <v>889</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
@@ -10136,13 +10136,13 @@
         <v>135</v>
       </c>
       <c r="E173" s="24" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="F173" s="24">
-        <v>890</v>
+        <v>1196</v>
       </c>
       <c r="G173" s="24">
-        <v>1195</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.2">
@@ -10159,13 +10159,13 @@
         <v>135</v>
       </c>
       <c r="E174" s="24" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="F174" s="24">
-        <v>1196</v>
+        <v>1877</v>
       </c>
       <c r="G174" s="24">
-        <v>1876</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.2">
@@ -10182,13 +10182,13 @@
         <v>135</v>
       </c>
       <c r="E175" s="24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F175" s="24">
-        <v>1877</v>
+        <v>2462</v>
       </c>
       <c r="G175" s="24">
-        <v>2461</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.2">
@@ -10205,13 +10205,13 @@
         <v>135</v>
       </c>
       <c r="E176" s="24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F176" s="24">
-        <v>2462</v>
+        <v>3584</v>
       </c>
       <c r="G176" s="24">
-        <v>3583</v>
+        <v>3793</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.2">
@@ -10228,13 +10228,13 @@
         <v>135</v>
       </c>
       <c r="E177" s="24" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="F177" s="24">
-        <v>3584</v>
+        <v>3794</v>
       </c>
       <c r="G177" s="24">
-        <v>3793</v>
+        <v>7471</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.2">
@@ -10251,13 +10251,13 @@
         <v>135</v>
       </c>
       <c r="E178" s="24" t="s">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="F178" s="24">
-        <v>3794</v>
+        <v>7472</v>
       </c>
       <c r="G178" s="24">
-        <v>7471</v>
+        <v>7663</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.2">
@@ -10274,13 +10274,13 @@
         <v>135</v>
       </c>
       <c r="E179" s="24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F179" s="24">
-        <v>7472</v>
+        <v>7664</v>
       </c>
       <c r="G179" s="24">
-        <v>7663</v>
+        <v>8704</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.2">
@@ -10297,13 +10297,13 @@
         <v>135</v>
       </c>
       <c r="E180" s="24" t="s">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="F180" s="24">
-        <v>7664</v>
+        <v>8705</v>
       </c>
       <c r="G180" s="24">
-        <v>8704</v>
+        <v>12349</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.2">
@@ -10320,13 +10320,13 @@
         <v>135</v>
       </c>
       <c r="E181" s="24" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="F181" s="24">
         <v>8705</v>
       </c>
       <c r="G181" s="24">
-        <v>12349</v>
+        <v>10192</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.2">
@@ -10343,13 +10343,13 @@
         <v>135</v>
       </c>
       <c r="E182" s="24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F182" s="24">
-        <v>8705</v>
+        <v>10193</v>
       </c>
       <c r="G182" s="24">
-        <v>10192</v>
+        <v>12349</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.2">
@@ -10366,36 +10366,36 @@
         <v>135</v>
       </c>
       <c r="E183" s="24" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F183" s="24">
-        <v>10193</v>
+        <v>12360</v>
       </c>
       <c r="G183" s="24">
-        <v>12349</v>
+        <v>12573</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" s="27" t="s">
-        <v>35</v>
+        <v>139</v>
       </c>
       <c r="B184" s="27" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C184" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D184" s="24" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E184" s="24" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="F184" s="24">
-        <v>12360</v>
+        <v>1</v>
       </c>
       <c r="G184" s="24">
-        <v>12573</v>
+        <v>12983</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.2">
@@ -10412,36 +10412,36 @@
         <v>136</v>
       </c>
       <c r="E185" s="24" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="F185" s="24">
-        <v>1</v>
+        <v>499</v>
       </c>
       <c r="G185" s="24">
-        <v>12983</v>
+        <v>12480</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" s="27" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B186" s="27" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C186" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D186" s="24" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E186" s="24" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="F186" s="24">
-        <v>499</v>
+        <v>1</v>
       </c>
       <c r="G186" s="24">
-        <v>12480</v>
+        <v>11276</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.2">
@@ -10458,36 +10458,36 @@
         <v>137</v>
       </c>
       <c r="E187" s="24" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="F187" s="24">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="G187" s="24">
-        <v>11276</v>
+        <v>11031</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B188" s="27" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C188" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D188" s="24" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E188" s="24" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="F188" s="24">
-        <v>124</v>
+        <v>1</v>
       </c>
       <c r="G188" s="24">
-        <v>11031</v>
+        <v>7797</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.2">
@@ -10504,36 +10504,34 @@
         <v>138</v>
       </c>
       <c r="E189" s="24" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="F189" s="24">
         <v>1</v>
       </c>
       <c r="G189" s="24">
-        <v>7797</v>
+        <v>7770</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A190" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="B190" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="C190" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D190" s="24" t="s">
-        <v>138</v>
-      </c>
+      <c r="A190" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B190" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="C190" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D190" s="24"/>
       <c r="E190" s="24" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="F190" s="24">
         <v>1</v>
       </c>
       <c r="G190" s="24">
-        <v>7770</v>
+        <v>10053</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.2">
@@ -10548,7 +10546,7 @@
       </c>
       <c r="D191" s="24"/>
       <c r="E191" s="24" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="F191" s="24">
         <v>1</v>
@@ -10569,13 +10567,13 @@
       </c>
       <c r="D192" s="24"/>
       <c r="E192" s="24" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="F192" s="24">
         <v>1</v>
       </c>
       <c r="G192" s="24">
-        <v>10053</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
@@ -10590,13 +10588,13 @@
       </c>
       <c r="D193" s="24"/>
       <c r="E193" s="24" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="F193" s="24">
         <v>1</v>
       </c>
       <c r="G193" s="24">
-        <v>2358</v>
+        <v>345</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
@@ -10611,13 +10609,13 @@
       </c>
       <c r="D194" s="24"/>
       <c r="E194" s="24" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="F194" s="24">
-        <v>1</v>
+        <v>346</v>
       </c>
       <c r="G194" s="24">
-        <v>345</v>
+        <v>852</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
@@ -10632,10 +10630,10 @@
       </c>
       <c r="D195" s="24"/>
       <c r="E195" s="24" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F195" s="24">
-        <v>346</v>
+        <v>655</v>
       </c>
       <c r="G195" s="24">
         <v>852</v>
@@ -10653,13 +10651,13 @@
       </c>
       <c r="D196" s="24"/>
       <c r="E196" s="24" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="F196" s="24">
-        <v>655</v>
+        <v>853</v>
       </c>
       <c r="G196" s="24">
-        <v>852</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
@@ -10674,13 +10672,13 @@
       </c>
       <c r="D197" s="24"/>
       <c r="E197" s="24" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="F197" s="24">
-        <v>853</v>
+        <v>2359</v>
       </c>
       <c r="G197" s="24">
-        <v>2358</v>
+        <v>10050</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
@@ -10695,13 +10693,13 @@
       </c>
       <c r="D198" s="24"/>
       <c r="E198" s="24" t="s">
-        <v>94</v>
+        <v>4</v>
       </c>
       <c r="F198" s="24">
         <v>2359</v>
       </c>
       <c r="G198" s="24">
-        <v>10050</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.2">
@@ -10716,13 +10714,13 @@
       </c>
       <c r="D199" s="24"/>
       <c r="E199" s="24" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="F199" s="24">
-        <v>2359</v>
+        <v>3391</v>
       </c>
       <c r="G199" s="24">
-        <v>3390</v>
+        <v>3978</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
@@ -10737,13 +10735,13 @@
       </c>
       <c r="D200" s="24"/>
       <c r="E200" s="24" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F200" s="24">
-        <v>3391</v>
+        <v>3979</v>
       </c>
       <c r="G200" s="24">
-        <v>3978</v>
+        <v>4431</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.2">
@@ -10758,13 +10756,13 @@
       </c>
       <c r="D201" s="24"/>
       <c r="E201" s="24" t="s">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="F201" s="24">
-        <v>3979</v>
+        <v>4432</v>
       </c>
       <c r="G201" s="24">
-        <v>4431</v>
+        <v>6303</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.2">
@@ -10779,13 +10777,13 @@
       </c>
       <c r="D202" s="24"/>
       <c r="E202" s="24" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="F202" s="24">
-        <v>4432</v>
+        <v>6304</v>
       </c>
       <c r="G202" s="24">
-        <v>6303</v>
+        <v>6687</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.2">
@@ -10800,13 +10798,13 @@
       </c>
       <c r="D203" s="24"/>
       <c r="E203" s="24" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="F203" s="24">
-        <v>6304</v>
+        <v>6688</v>
       </c>
       <c r="G203" s="24">
-        <v>6687</v>
+        <v>6762</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.2">
@@ -10821,13 +10819,13 @@
       </c>
       <c r="D204" s="24"/>
       <c r="E204" s="24" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="F204" s="24">
-        <v>6688</v>
+        <v>6763</v>
       </c>
       <c r="G204" s="24">
-        <v>6762</v>
+        <v>7557</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
@@ -10842,36 +10840,36 @@
       </c>
       <c r="D205" s="24"/>
       <c r="E205" s="24" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="F205" s="24">
-        <v>6763</v>
+        <v>7558</v>
       </c>
       <c r="G205" s="24">
-        <v>7557</v>
-      </c>
+        <v>10050</v>
+      </c>
+      <c r="H205" s="22"/>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" s="24" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="B206" s="24" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C206" s="24" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="D206" s="24"/>
-      <c r="E206" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F206" s="24">
-        <v>7558</v>
-      </c>
-      <c r="G206" s="24">
-        <v>10050</v>
-      </c>
-      <c r="H206" s="22"/>
+      <c r="E206" t="s">
+        <v>72</v>
+      </c>
+      <c r="F206">
+        <v>1</v>
+      </c>
+      <c r="G206">
+        <v>5938</v>
+      </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" s="24" t="s">
@@ -10884,14 +10882,14 @@
         <v>96</v>
       </c>
       <c r="D207" s="24"/>
-      <c r="E207" t="s">
-        <v>72</v>
-      </c>
-      <c r="F207">
-        <v>1</v>
-      </c>
-      <c r="G207">
-        <v>5938</v>
+      <c r="E207" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F207" s="24">
+        <v>117</v>
+      </c>
+      <c r="G207" s="24">
+        <v>2543</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.2">
@@ -10906,35 +10904,35 @@
       </c>
       <c r="D208" s="24"/>
       <c r="E208" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="F208" s="24">
-        <v>117</v>
+        <v>114</v>
+      </c>
+      <c r="F208">
+        <f t="shared" ref="F208" si="0">(D208+2824)</f>
+        <v>2824</v>
       </c>
       <c r="G208" s="24">
-        <v>2543</v>
+        <v>5673</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209" s="24" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B209" s="24" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C209" s="24" t="s">
         <v>96</v>
       </c>
       <c r="D209" s="24"/>
-      <c r="E209" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="F209">
-        <f t="shared" ref="F209" si="0">(D209+2824)</f>
-        <v>2824</v>
+      <c r="E209" t="s">
+        <v>72</v>
+      </c>
+      <c r="F209" s="24">
+        <v>1</v>
       </c>
       <c r="G209" s="24">
-        <v>5673</v>
+        <v>3114</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.2">
@@ -10948,35 +10946,35 @@
         <v>96</v>
       </c>
       <c r="D210" s="24"/>
-      <c r="E210" t="s">
-        <v>72</v>
-      </c>
-      <c r="F210" s="24">
-        <v>1</v>
-      </c>
-      <c r="G210" s="24">
-        <v>3114</v>
+      <c r="E210" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="F210">
+        <v>105</v>
+      </c>
+      <c r="G210">
+        <v>2849</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211" s="24" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B211" s="24" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C211" s="24" t="s">
         <v>96</v>
       </c>
       <c r="D211" s="24"/>
-      <c r="E211" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="F211">
-        <v>105</v>
-      </c>
-      <c r="G211">
-        <v>2849</v>
+      <c r="E211" t="s">
+        <v>72</v>
+      </c>
+      <c r="F211" s="24">
+        <v>1</v>
+      </c>
+      <c r="G211" s="24">
+        <v>2824</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.2">
@@ -10990,40 +10988,24 @@
         <v>96</v>
       </c>
       <c r="D212" s="24"/>
-      <c r="E212" t="s">
-        <v>72</v>
-      </c>
-      <c r="F212" s="24">
-        <v>1</v>
-      </c>
-      <c r="G212" s="24">
-        <v>2824</v>
-      </c>
-    </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A213" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="B213" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="C213" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="D213" s="24"/>
-      <c r="E213" s="24" t="s">
+      <c r="E212" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="F213">
+      <c r="F212">
         <v>117</v>
       </c>
-      <c r="G213">
+      <c r="G212">
         <v>2543</v>
       </c>
+    </row>
+    <row r="247" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B247" s="1"/>
+      <c r="C247" s="5"/>
     </row>
     <row r="248" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B248" s="1"/>
       <c r="C248" s="5"/>
+      <c r="D248" s="5"/>
     </row>
     <row r="249" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B249" s="1"/>
@@ -11137,16 +11119,16 @@
     </row>
     <row r="271" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B271" s="1"/>
-      <c r="C271" s="5"/>
       <c r="D271" s="5"/>
     </row>
     <row r="272" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B272" s="1"/>
-      <c r="D272" s="5"/>
+      <c r="C272" s="5"/>
     </row>
     <row r="273" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B273" s="1"/>
       <c r="C273" s="5"/>
+      <c r="D273" s="5"/>
     </row>
     <row r="274" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B274" s="1"/>
@@ -11174,27 +11156,27 @@
       <c r="D278" s="5"/>
     </row>
     <row r="279" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B279" s="1"/>
-      <c r="C279" s="5"/>
       <c r="D279" s="5"/>
     </row>
-    <row r="280" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D280" s="5"/>
-    </row>
-    <row r="962" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C962"/>
-      <c r="D962"/>
-      <c r="E962" s="1"/>
+    <row r="961" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C961"/>
+      <c r="D961"/>
+      <c r="E961" s="1"/>
+    </row>
+    <row r="1097" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1097" s="1"/>
+      <c r="C1097"/>
+      <c r="D1097"/>
     </row>
     <row r="1098" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1098" s="1"/>
       <c r="C1098"/>
       <c r="D1098"/>
     </row>
-    <row r="1099" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1099" s="1"/>
-      <c r="C1099"/>
-      <c r="D1099"/>
+    <row r="1223" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1223" s="1"/>
+      <c r="C1223"/>
+      <c r="D1223"/>
     </row>
     <row r="1224" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1224" s="1"/>
@@ -11221,10 +11203,9 @@
       <c r="C1228"/>
       <c r="D1228"/>
     </row>
-    <row r="1229" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1229" s="1"/>
-      <c r="C1229"/>
-      <c r="D1229"/>
+    <row r="1273" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E1273" s="1"/>
+      <c r="F1273" s="1"/>
     </row>
     <row r="1274" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E1274" s="1"/>
@@ -11234,9 +11215,8 @@
       <c r="E1275" s="1"/>
       <c r="F1275" s="1"/>
     </row>
-    <row r="1276" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E1276" s="1"/>
-      <c r="F1276" s="1"/>
+    <row r="1277" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1277" s="1"/>
     </row>
     <row r="1278" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1278" s="1"/>
@@ -11250,8 +11230,10 @@
     <row r="1281" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1281" s="1"/>
     </row>
-    <row r="1282" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1282" s="1"/>
+    <row r="1300" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1300" s="1"/>
+      <c r="C1300"/>
+      <c r="D1300"/>
     </row>
     <row r="1301" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1301" s="1"/>
@@ -11283,10 +11265,10 @@
       <c r="C1306"/>
       <c r="D1306"/>
     </row>
-    <row r="1307" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1307" s="1"/>
-      <c r="C1307"/>
-      <c r="D1307"/>
+    <row r="1308" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1308" s="1"/>
+      <c r="C1308"/>
+      <c r="D1308"/>
     </row>
     <row r="1309" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1309" s="1"/>
@@ -11313,10 +11295,10 @@
       <c r="C1313"/>
       <c r="D1313"/>
     </row>
-    <row r="1314" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1314" s="1"/>
-      <c r="C1314"/>
-      <c r="D1314"/>
+    <row r="1365" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1365" s="1"/>
+      <c r="C1365"/>
+      <c r="D1365"/>
     </row>
     <row r="1366" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1366" s="1"/>
@@ -11333,10 +11315,10 @@
       <c r="C1368"/>
       <c r="D1368"/>
     </row>
-    <row r="1369" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1369" s="1"/>
-      <c r="C1369"/>
-      <c r="D1369"/>
+    <row r="1370" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1370" s="1"/>
+      <c r="C1370"/>
+      <c r="D1370"/>
     </row>
     <row r="1371" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1371" s="1"/>
@@ -11353,10 +11335,10 @@
       <c r="C1373"/>
       <c r="D1373"/>
     </row>
-    <row r="1374" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1374" s="1"/>
-      <c r="C1374"/>
-      <c r="D1374"/>
+    <row r="1408" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1408" s="1"/>
+      <c r="C1408"/>
+      <c r="D1408"/>
     </row>
     <row r="1409" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1409" s="1"/>
@@ -11383,17 +11365,18 @@
       <c r="C1413"/>
       <c r="D1413"/>
     </row>
-    <row r="1414" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1414" s="1"/>
-      <c r="C1414"/>
-      <c r="D1414"/>
-    </row>
-    <row r="1456" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="1455" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="E1455" s="1"/>
+      <c r="F1455" s="1"/>
+    </row>
+    <row r="1456" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C1456" s="6"/>
       <c r="E1456" s="1"/>
       <c r="F1456" s="1"/>
     </row>
     <row r="1457" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C1457" s="6"/>
+      <c r="D1457" s="6"/>
       <c r="E1457" s="1"/>
       <c r="F1457" s="1"/>
     </row>
@@ -11404,15 +11387,14 @@
       <c r="F1458" s="1"/>
     </row>
     <row r="1459" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C1459" s="6"/>
       <c r="D1459" s="6"/>
       <c r="E1459" s="1"/>
       <c r="F1459" s="1"/>
     </row>
-    <row r="1460" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D1460" s="6"/>
-      <c r="E1460" s="1"/>
-      <c r="F1460" s="1"/>
+    <row r="1522" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1522" s="1"/>
+      <c r="C1522"/>
+      <c r="D1522"/>
     </row>
     <row r="1523" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1523" s="1"/>
@@ -11429,15 +11411,10 @@
       <c r="C1525"/>
       <c r="D1525"/>
     </row>
-    <row r="1526" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1526" s="1"/>
-      <c r="C1526"/>
-      <c r="D1526"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G1479">
-    <sortCondition ref="C2:C1479"/>
-    <sortCondition ref="D2:D1479"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G1478">
+    <sortCondition ref="C2:C1478"/>
+    <sortCondition ref="D2:D1478"/>
   </sortState>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated master reference for Hepaci subgroup 2
</commit_message>
<xml_diff>
--- a/tabular/core/flavi-reference_feature_locations.xlsx
+++ b/tabular/core/flavi-reference_feature_locations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flavivirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4F868D-5EFA-0047-AD4E-97E924888D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB21716-7580-9041-9BB6-D9D8B21A4B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18500" yWindow="1120" windowWidth="34460" windowHeight="22160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16740" yWindow="1120" windowWidth="34460" windowHeight="22160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="175">
   <si>
     <t>featureName</t>
   </si>
@@ -555,6 +555,15 @@
   </si>
   <si>
     <t>REF_MASTER_HEPACI_2_GBVB</t>
+  </si>
+  <si>
+    <t>NC_001656</t>
+  </si>
+  <si>
+    <t>NC_001657</t>
+  </si>
+  <si>
+    <t>NC_001658</t>
   </si>
 </sst>
 </file>
@@ -6189,10 +6198,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1531"/>
+  <dimension ref="A1:H1540"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E128" sqref="A1:G233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9020,20 +9029,20 @@
       <c r="B123" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="C123" s="59" t="s">
+      <c r="C123" s="58" t="s">
         <v>21</v>
       </c>
       <c r="D123" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="E123" s="17" t="s">
-        <v>86</v>
+      <c r="E123" s="30" t="s">
+        <v>22</v>
       </c>
       <c r="F123" s="17">
-        <v>914</v>
+        <v>446</v>
       </c>
       <c r="G123" s="17">
-        <v>1492</v>
+        <v>913</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
@@ -9050,497 +9059,510 @@
         <v>119</v>
       </c>
       <c r="E124" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F124" s="17">
+        <v>914</v>
+      </c>
+      <c r="G124" s="17">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A125" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="B125" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="C125" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="D125" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="E125" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F124" s="17">
+      <c r="F125" s="17">
         <v>1493</v>
       </c>
-      <c r="G124" s="6">
+      <c r="G125" s="17">
         <v>2452</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A125" s="58" t="s">
-        <v>120</v>
-      </c>
-      <c r="B125" s="58" t="s">
-        <v>150</v>
-      </c>
-      <c r="C125" s="58" t="s">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A126" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="B126" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="C126" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="D125" s="36" t="s">
+      <c r="D126" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="E126" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F126" s="17">
+        <v>2456</v>
+      </c>
+      <c r="G126" s="17">
+        <v>2641</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A127" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="B127" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="C127" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="D127" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="E127" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F127" s="17">
+        <v>2642</v>
+      </c>
+      <c r="G127" s="17">
+        <v>3265</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A128" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="B128" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="C128" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="D128" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="E128" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F128" s="17">
+        <v>3266</v>
+      </c>
+      <c r="G128" s="17">
+        <v>5125</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A129" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="B129" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="C129" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="D129" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="E129" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="F129" s="17">
+        <v>5126</v>
+      </c>
+      <c r="G129" s="17">
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A130" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="B130" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="C130" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="D130" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="E130" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F130" s="17">
+        <v>5291</v>
+      </c>
+      <c r="G130" s="17">
+        <v>6034</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A131" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="B131" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="C131" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="D131" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="E125" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="F125" s="30">
-        <v>1</v>
-      </c>
-      <c r="G125" s="30">
-        <v>9609</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A126" s="58" t="s">
-        <v>120</v>
-      </c>
-      <c r="B126" s="58" t="s">
-        <v>150</v>
-      </c>
-      <c r="C126" s="58" t="s">
+      <c r="E131" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F131" s="17">
+        <v>6035</v>
+      </c>
+      <c r="G131" s="17">
+        <v>9037</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A132" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="B132" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="C132" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="D126" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="E126" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F126" s="30">
-        <v>281</v>
-      </c>
-      <c r="G126" s="30">
-        <v>9355</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A127" s="58" t="s">
-        <v>123</v>
-      </c>
-      <c r="B127" s="58" t="s">
-        <v>151</v>
-      </c>
-      <c r="C127" s="58" t="s">
+      <c r="D132" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="E132" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F132" s="17">
+        <v>6035</v>
+      </c>
+      <c r="G132" s="17">
+        <v>7267</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A133" s="59" t="s">
+        <v>174</v>
+      </c>
+      <c r="B133" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="C133" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="D127" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="E127" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="F127" s="30">
-        <v>1</v>
-      </c>
-      <c r="G127" s="30">
-        <v>9687</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A128" s="58" t="s">
-        <v>123</v>
-      </c>
-      <c r="B128" s="58" t="s">
-        <v>151</v>
-      </c>
-      <c r="C128" s="58" t="s">
-        <v>21</v>
-      </c>
-      <c r="D128" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="E128" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F128" s="30">
-        <v>558</v>
-      </c>
-      <c r="G128" s="30">
-        <v>9602</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A129" s="58" t="s">
-        <v>124</v>
-      </c>
-      <c r="B129" s="58" t="s">
-        <v>152</v>
-      </c>
-      <c r="C129" s="58" t="s">
-        <v>21</v>
-      </c>
-      <c r="D129" s="36" t="s">
+      <c r="D133" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="E129" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="F129" s="30">
-        <v>1</v>
-      </c>
-      <c r="G129" s="30">
-        <v>11013</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A130" s="58" t="s">
-        <v>124</v>
-      </c>
-      <c r="B130" s="58" t="s">
-        <v>152</v>
-      </c>
-      <c r="C130" s="58" t="s">
-        <v>21</v>
-      </c>
-      <c r="D130" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="E130" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F130" s="30">
-        <v>578</v>
-      </c>
-      <c r="G130" s="30">
-        <v>10870</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A131" s="58" t="s">
-        <v>125</v>
-      </c>
-      <c r="B131" s="58" t="s">
-        <v>153</v>
-      </c>
-      <c r="C131" s="58" t="s">
-        <v>21</v>
-      </c>
-      <c r="D131" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="E131" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="F131" s="30">
-        <v>1</v>
-      </c>
-      <c r="G131" s="30">
-        <v>10199</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A132" s="58" t="s">
-        <v>125</v>
-      </c>
-      <c r="B132" s="58" t="s">
-        <v>153</v>
-      </c>
-      <c r="C132" s="58" t="s">
-        <v>21</v>
-      </c>
-      <c r="D132" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="E132" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F132" s="30">
-        <v>3</v>
-      </c>
-      <c r="G132" s="30">
-        <v>10127</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A133" s="58" t="s">
-        <v>129</v>
-      </c>
-      <c r="B133" s="58" t="s">
-        <v>154</v>
-      </c>
-      <c r="C133" s="58" t="s">
-        <v>21</v>
-      </c>
-      <c r="D133" s="36" t="s">
-        <v>128</v>
-      </c>
       <c r="E133" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="F133" s="30">
-        <v>1</v>
-      </c>
-      <c r="G133" s="30">
-        <v>10272</v>
+        <v>25</v>
+      </c>
+      <c r="F133" s="17">
+        <v>7268</v>
+      </c>
+      <c r="G133" s="17">
+        <v>9037</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" s="58" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B134" s="58" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C134" s="58" t="s">
         <v>21</v>
       </c>
       <c r="D134" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="E134" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F134" s="30">
-        <v>174</v>
-      </c>
-      <c r="G134" s="30">
-        <v>10241</v>
+        <v>121</v>
+      </c>
+      <c r="E134" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F134" s="17">
+        <v>1</v>
+      </c>
+      <c r="G134" s="17">
+        <v>9609</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" s="58" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B135" s="58" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C135" s="58" t="s">
         <v>21</v>
       </c>
       <c r="D135" s="36" t="s">
-        <v>130</v>
-      </c>
-      <c r="E135" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="F135" s="30">
-        <v>1</v>
-      </c>
-      <c r="G135" s="30">
-        <v>8697</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" ht="17" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="E135" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F135" s="17">
+        <v>281</v>
+      </c>
+      <c r="G135" s="17">
+        <v>9355</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="58" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B136" s="58" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C136" s="58" t="s">
         <v>21</v>
       </c>
       <c r="D136" s="36" t="s">
-        <v>130</v>
-      </c>
-      <c r="E136" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F136" s="30">
+        <v>122</v>
+      </c>
+      <c r="E136" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F136" s="17">
         <v>1</v>
       </c>
-      <c r="G136" s="37">
-        <v>8622</v>
+      <c r="G136" s="17">
+        <v>9687</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="58" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B137" s="58" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C137" s="58" t="s">
         <v>21</v>
       </c>
       <c r="D137" s="36" t="s">
-        <v>131</v>
-      </c>
-      <c r="E137" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="F137" s="30">
-        <v>1</v>
-      </c>
-      <c r="G137" s="30">
-        <v>9653</v>
+        <v>122</v>
+      </c>
+      <c r="E137" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F137" s="17">
+        <v>558</v>
+      </c>
+      <c r="G137" s="17">
+        <v>9602</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="58" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B138" s="58" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C138" s="58" t="s">
         <v>21</v>
       </c>
       <c r="D138" s="36" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E138" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="F138" s="30">
+        <v>1</v>
+      </c>
+      <c r="G138" s="30">
+        <v>11013</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A139" s="58" t="s">
+        <v>124</v>
+      </c>
+      <c r="B139" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="C139" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D139" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="E139" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="F138" s="30">
-        <v>132</v>
-      </c>
-      <c r="G138" s="30">
-        <v>9392</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A139" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="B139" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="C139" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D139" s="30"/>
-      <c r="E139" s="40" t="s">
+      <c r="F139" s="30">
+        <v>578</v>
+      </c>
+      <c r="G139" s="30">
+        <v>10870</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A140" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="B140" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="C140" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D140" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="E140" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="F139" s="40">
+      <c r="F140" s="30">
         <v>1</v>
       </c>
-      <c r="G139" s="40">
-        <v>5938</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A140" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="B140" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="C140" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D140" s="30"/>
-      <c r="E140" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="F140" s="30">
-        <v>117</v>
-      </c>
       <c r="G140" s="30">
-        <v>2543</v>
+        <v>10199</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A141" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="B141" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="C141" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D141" s="30"/>
+      <c r="A141" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="B141" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="C141" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D141" s="36" t="s">
+        <v>127</v>
+      </c>
       <c r="E141" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="F141" s="40">
-        <f>(D141+2824)</f>
-        <v>2824</v>
+        <v>61</v>
+      </c>
+      <c r="F141" s="30">
+        <v>3</v>
       </c>
       <c r="G141" s="30">
-        <v>5673</v>
+        <v>10127</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A142" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="B142" s="30" t="s">
-        <v>166</v>
-      </c>
-      <c r="C142" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D142" s="30"/>
-      <c r="E142" s="40" t="s">
+      <c r="A142" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B142" s="58" t="s">
+        <v>154</v>
+      </c>
+      <c r="C142" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D142" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="E142" s="30" t="s">
         <v>72</v>
       </c>
       <c r="F142" s="30">
         <v>1</v>
       </c>
       <c r="G142" s="30">
-        <v>3114</v>
+        <v>10272</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A143" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="B143" s="30" t="s">
-        <v>166</v>
-      </c>
-      <c r="C143" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D143" s="30"/>
+      <c r="A143" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B143" s="58" t="s">
+        <v>154</v>
+      </c>
+      <c r="C143" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D143" s="36" t="s">
+        <v>128</v>
+      </c>
       <c r="E143" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="F143" s="40">
-        <v>105</v>
-      </c>
-      <c r="G143" s="40">
-        <v>2849</v>
+        <v>61</v>
+      </c>
+      <c r="F143" s="30">
+        <v>174</v>
+      </c>
+      <c r="G143" s="30">
+        <v>10241</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A144" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="B144" s="30" t="s">
-        <v>167</v>
-      </c>
-      <c r="C144" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D144" s="30"/>
-      <c r="E144" s="40" t="s">
+      <c r="A144" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="B144" s="58" t="s">
+        <v>155</v>
+      </c>
+      <c r="C144" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D144" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="E144" s="30" t="s">
         <v>72</v>
       </c>
       <c r="F144" s="30">
         <v>1</v>
       </c>
       <c r="G144" s="30">
-        <v>2824</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A145" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="B145" s="30" t="s">
-        <v>167</v>
-      </c>
-      <c r="C145" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D145" s="30"/>
+        <v>8697</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="17" x14ac:dyDescent="0.25">
+      <c r="A145" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="B145" s="58" t="s">
+        <v>155</v>
+      </c>
+      <c r="C145" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D145" s="36" t="s">
+        <v>130</v>
+      </c>
       <c r="E145" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="F145" s="40">
-        <v>117</v>
-      </c>
-      <c r="G145" s="40">
-        <v>2543</v>
+        <v>61</v>
+      </c>
+      <c r="F145" s="30">
+        <v>1</v>
+      </c>
+      <c r="G145" s="37">
+        <v>8622</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A146" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="B146" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="C146" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="D146" s="38" t="s">
-        <v>141</v>
+      <c r="A146" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B146" s="58" t="s">
+        <v>156</v>
+      </c>
+      <c r="C146" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D146" s="36" t="s">
+        <v>131</v>
       </c>
       <c r="E146" s="30" t="s">
         <v>72</v>
@@ -9549,191 +9571,178 @@
         <v>1</v>
       </c>
       <c r="G146" s="30">
-        <v>9867</v>
+        <v>9653</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A147" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="B147" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="C147" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="D147" s="38" t="s">
-        <v>141</v>
+      <c r="A147" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B147" s="58" t="s">
+        <v>156</v>
+      </c>
+      <c r="C147" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D147" s="36" t="s">
+        <v>131</v>
       </c>
       <c r="E147" s="30" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="F147" s="30">
+        <v>132</v>
+      </c>
+      <c r="G147" s="30">
+        <v>9392</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A148" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B148" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="C148" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D148" s="30"/>
+      <c r="E148" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="F148" s="40">
         <v>1</v>
       </c>
-      <c r="G147" s="30">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A148" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="B148" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="C148" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="D148" s="38" t="s">
-        <v>141</v>
-      </c>
-      <c r="E148" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F148" s="30">
-        <v>328</v>
-      </c>
-      <c r="G148" s="30">
-        <v>9501</v>
+      <c r="G148" s="40">
+        <v>5938</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A149" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="B149" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="C149" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="D149" s="38" t="s">
-        <v>141</v>
-      </c>
+      <c r="A149" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B149" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="C149" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D149" s="30"/>
       <c r="E149" s="30" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="F149" s="30">
-        <v>328</v>
+        <v>117</v>
       </c>
       <c r="G149" s="30">
-        <v>2199</v>
+        <v>2543</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A150" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="B150" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="C150" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="D150" s="38" t="s">
-        <v>141</v>
-      </c>
+      <c r="A150" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B150" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="C150" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D150" s="30"/>
       <c r="E150" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="F150" s="30">
-        <v>328</v>
+        <v>114</v>
+      </c>
+      <c r="F150" s="40">
+        <f>(D150+2824)</f>
+        <v>2824</v>
       </c>
       <c r="G150" s="30">
-        <v>564</v>
+        <v>5673</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A151" s="61" t="s">
-        <v>37</v>
-      </c>
-      <c r="B151" s="61" t="s">
-        <v>157</v>
-      </c>
-      <c r="C151" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="D151" s="45" t="s">
-        <v>141</v>
-      </c>
-      <c r="E151" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="F151" s="17">
-        <v>523</v>
-      </c>
-      <c r="G151" s="17">
-        <v>1137</v>
+      <c r="A151" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B151" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="C151" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D151" s="30"/>
+      <c r="E151" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="F151" s="30">
+        <v>1</v>
+      </c>
+      <c r="G151" s="30">
+        <v>3114</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A152" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="B152" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="C152" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="D152" s="38" t="s">
-        <v>141</v>
-      </c>
+      <c r="A152" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B152" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="C152" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D152" s="30"/>
       <c r="E152" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="F152" s="30">
-        <v>1138</v>
-      </c>
-      <c r="G152" s="30">
-        <v>2199</v>
+        <v>114</v>
+      </c>
+      <c r="F152" s="40">
+        <v>105</v>
+      </c>
+      <c r="G152" s="40">
+        <v>2849</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A153" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="B153" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="C153" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="D153" s="38" t="s">
-        <v>141</v>
-      </c>
-      <c r="E153" s="30" t="s">
-        <v>68</v>
+      <c r="A153" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="B153" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="C153" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D153" s="30"/>
+      <c r="E153" s="40" t="s">
+        <v>72</v>
       </c>
       <c r="F153" s="30">
-        <v>2200</v>
+        <v>1</v>
       </c>
       <c r="G153" s="30">
-        <v>2910</v>
+        <v>2824</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A154" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="B154" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="C154" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="D154" s="38" t="s">
-        <v>141</v>
-      </c>
+      <c r="A154" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="B154" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="C154" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D154" s="30"/>
       <c r="E154" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="F154" s="30">
-        <v>2911</v>
-      </c>
-      <c r="G154" s="30">
-        <v>9498</v>
+        <v>103</v>
+      </c>
+      <c r="F154" s="40">
+        <v>117</v>
+      </c>
+      <c r="G154" s="40">
+        <v>2543</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
@@ -9750,13 +9759,13 @@
         <v>141</v>
       </c>
       <c r="E155" s="30" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="F155" s="30">
-        <v>2911</v>
+        <v>1</v>
       </c>
       <c r="G155" s="30">
-        <v>3630</v>
+        <v>9867</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
@@ -9773,13 +9782,13 @@
         <v>141</v>
       </c>
       <c r="E156" s="30" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F156" s="30">
-        <v>3631</v>
+        <v>1</v>
       </c>
       <c r="G156" s="30">
-        <v>5514</v>
+        <v>327</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
@@ -9796,13 +9805,13 @@
         <v>141</v>
       </c>
       <c r="E157" s="30" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="F157" s="30">
-        <v>5515</v>
+        <v>328</v>
       </c>
       <c r="G157" s="30">
-        <v>5637</v>
+        <v>9501</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
@@ -9819,13 +9828,13 @@
         <v>141</v>
       </c>
       <c r="E158" s="30" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F158" s="30">
-        <v>5638</v>
+        <v>328</v>
       </c>
       <c r="G158" s="30">
-        <v>6423</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
@@ -9842,36 +9851,36 @@
         <v>141</v>
       </c>
       <c r="E159" s="30" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="F159" s="30">
-        <v>6424</v>
+        <v>328</v>
       </c>
       <c r="G159" s="30">
-        <v>9498</v>
+        <v>564</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A160" s="60" t="s">
+      <c r="A160" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="B160" s="60" t="s">
+      <c r="B160" s="61" t="s">
         <v>157</v>
       </c>
-      <c r="C160" s="60" t="s">
+      <c r="C160" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="D160" s="38" t="s">
+      <c r="D160" s="45" t="s">
         <v>141</v>
       </c>
-      <c r="E160" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="F160" s="30">
-        <v>6424</v>
-      </c>
-      <c r="G160" s="30">
-        <v>7797</v>
+      <c r="E160" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F160" s="17">
+        <v>523</v>
+      </c>
+      <c r="G160" s="17">
+        <v>1137</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
@@ -9888,13 +9897,13 @@
         <v>141</v>
       </c>
       <c r="E161" s="30" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="F161" s="30">
-        <v>7798</v>
+        <v>1138</v>
       </c>
       <c r="G161" s="30">
-        <v>9498</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.2">
@@ -9911,220 +9920,220 @@
         <v>141</v>
       </c>
       <c r="E162" s="30" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="F162" s="30">
-        <v>9502</v>
+        <v>2200</v>
       </c>
       <c r="G162" s="30">
-        <v>9867</v>
+        <v>2910</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" s="60" t="s">
-        <v>116</v>
+        <v>37</v>
       </c>
       <c r="B163" s="60" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C163" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="D163" s="39" t="s">
-        <v>142</v>
+      <c r="D163" s="38" t="s">
+        <v>141</v>
       </c>
       <c r="E163" s="30" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="F163" s="30">
-        <v>1</v>
+        <v>2911</v>
       </c>
       <c r="G163" s="30">
-        <v>10479</v>
+        <v>9498</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" s="60" t="s">
-        <v>116</v>
+        <v>37</v>
       </c>
       <c r="B164" s="60" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C164" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="D164" s="39" t="s">
-        <v>142</v>
+      <c r="D164" s="38" t="s">
+        <v>141</v>
       </c>
       <c r="E164" s="30" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="F164" s="30">
-        <v>1</v>
+        <v>2911</v>
       </c>
       <c r="G164" s="30">
-        <v>617</v>
+        <v>3630</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" s="60" t="s">
-        <v>116</v>
+        <v>37</v>
       </c>
       <c r="B165" s="60" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C165" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="D165" s="39" t="s">
-        <v>142</v>
+      <c r="D165" s="38" t="s">
+        <v>141</v>
       </c>
       <c r="E165" s="30" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="F165" s="30">
-        <v>618</v>
+        <v>3631</v>
       </c>
       <c r="G165" s="30">
-        <v>10187</v>
+        <v>5514</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" s="60" t="s">
-        <v>116</v>
+        <v>37</v>
       </c>
       <c r="B166" s="60" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C166" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="D166" s="39" t="s">
-        <v>142</v>
+      <c r="D166" s="38" t="s">
+        <v>141</v>
       </c>
       <c r="E166" s="30" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="F166" s="30">
-        <v>618</v>
+        <v>5515</v>
       </c>
       <c r="G166" s="30">
-        <v>695</v>
+        <v>5637</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A167" s="61" t="s">
-        <v>116</v>
-      </c>
-      <c r="B167" s="61" t="s">
-        <v>158</v>
-      </c>
-      <c r="C167" s="61" t="s">
+      <c r="A167" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="B167" s="60" t="s">
+        <v>157</v>
+      </c>
+      <c r="C167" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="D167" s="46" t="s">
-        <v>142</v>
-      </c>
-      <c r="E167" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="F167" s="17">
-        <v>678</v>
-      </c>
-      <c r="G167" s="17">
-        <v>1235</v>
+      <c r="D167" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="E167" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F167" s="30">
+        <v>5638</v>
+      </c>
+      <c r="G167" s="30">
+        <v>6423</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A168" s="61" t="s">
-        <v>116</v>
-      </c>
-      <c r="B168" s="61" t="s">
-        <v>158</v>
-      </c>
-      <c r="C168" s="61" t="s">
+      <c r="A168" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="B168" s="60" t="s">
+        <v>157</v>
+      </c>
+      <c r="C168" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="D168" s="46" t="s">
-        <v>142</v>
-      </c>
-      <c r="E168" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="F168" s="17">
-        <v>1236</v>
-      </c>
-      <c r="G168" s="17">
-        <v>2180</v>
+      <c r="D168" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="E168" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F168" s="30">
+        <v>6424</v>
+      </c>
+      <c r="G168" s="30">
+        <v>9498</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" s="60" t="s">
-        <v>116</v>
+        <v>37</v>
       </c>
       <c r="B169" s="60" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C169" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="D169" s="39" t="s">
-        <v>142</v>
+      <c r="D169" s="38" t="s">
+        <v>141</v>
       </c>
       <c r="E169" s="30" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="F169" s="30">
-        <v>2784</v>
+        <v>6424</v>
       </c>
       <c r="G169" s="30">
-        <v>3449</v>
+        <v>7797</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" s="60" t="s">
-        <v>116</v>
+        <v>37</v>
       </c>
       <c r="B170" s="60" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C170" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="D170" s="39" t="s">
-        <v>142</v>
+      <c r="D170" s="38" t="s">
+        <v>141</v>
       </c>
       <c r="E170" s="30" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F170" s="30">
-        <v>3450</v>
+        <v>7798</v>
       </c>
       <c r="G170" s="30">
-        <v>5324</v>
+        <v>9498</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" s="60" t="s">
-        <v>116</v>
+        <v>37</v>
       </c>
       <c r="B171" s="60" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C171" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="D171" s="39" t="s">
-        <v>142</v>
+      <c r="D171" s="38" t="s">
+        <v>141</v>
       </c>
       <c r="E171" s="30" t="s">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="F171" s="30">
-        <v>5325</v>
+        <v>9502</v>
       </c>
       <c r="G171" s="30">
-        <v>5591</v>
+        <v>9867</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.2">
@@ -10141,13 +10150,13 @@
         <v>142</v>
       </c>
       <c r="E172" s="30" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="F172" s="30">
-        <v>5592</v>
+        <v>1</v>
       </c>
       <c r="G172" s="30">
-        <v>6422</v>
+        <v>10479</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
@@ -10164,13 +10173,13 @@
         <v>142</v>
       </c>
       <c r="E173" s="30" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F173" s="30">
-        <v>8388</v>
+        <v>1</v>
       </c>
       <c r="G173" s="30">
-        <v>10184</v>
+        <v>617</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.2">
@@ -10187,381 +10196,381 @@
         <v>142</v>
       </c>
       <c r="E174" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="F174" s="30">
+        <v>618</v>
+      </c>
+      <c r="G174" s="30">
+        <v>10187</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A175" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="B175" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="C175" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="D175" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="E175" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="F175" s="30">
+        <v>618</v>
+      </c>
+      <c r="G175" s="30">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A176" s="61" t="s">
+        <v>116</v>
+      </c>
+      <c r="B176" s="61" t="s">
+        <v>158</v>
+      </c>
+      <c r="C176" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="D176" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="E176" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F176" s="17">
+        <v>678</v>
+      </c>
+      <c r="G176" s="17">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A177" s="61" t="s">
+        <v>116</v>
+      </c>
+      <c r="B177" s="61" t="s">
+        <v>158</v>
+      </c>
+      <c r="C177" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="D177" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="E177" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F177" s="17">
+        <v>1236</v>
+      </c>
+      <c r="G177" s="17">
+        <v>2180</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A178" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="B178" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="C178" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="D178" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="E178" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="F178" s="30">
+        <v>2784</v>
+      </c>
+      <c r="G178" s="30">
+        <v>3449</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A179" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="B179" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="C179" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="D179" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="E179" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F179" s="30">
+        <v>3450</v>
+      </c>
+      <c r="G179" s="30">
+        <v>5324</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A180" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="B180" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="C180" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="D180" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="E180" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="F180" s="30">
+        <v>5325</v>
+      </c>
+      <c r="G180" s="30">
+        <v>5591</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A181" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="B181" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="C181" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="D181" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="E181" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F181" s="30">
+        <v>5592</v>
+      </c>
+      <c r="G181" s="30">
+        <v>6422</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A182" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="B182" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="C182" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="D182" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="E182" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F182" s="30">
+        <v>8388</v>
+      </c>
+      <c r="G182" s="30">
+        <v>10184</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A183" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="B183" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="C183" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="D183" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="E183" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F174" s="30">
+      <c r="F183" s="30">
         <v>10188</v>
       </c>
-      <c r="G174" s="30">
+      <c r="G183" s="30">
         <v>10479</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A175" s="40" t="s">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A184" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="B175" s="40" t="s">
+      <c r="B184" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="C175" s="41" t="s">
+      <c r="C184" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="D175" s="42" t="s">
+      <c r="D184" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="E175" s="30" t="s">
+      <c r="E184" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="F175" s="30">
+      <c r="F184" s="30">
         <v>1</v>
       </c>
-      <c r="G175" s="30">
+      <c r="G184" s="30">
         <v>10861</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A176" s="40" t="s">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A185" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="B176" s="40" t="s">
+      <c r="B185" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="C176" s="41" t="s">
+      <c r="C185" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="D176" s="42" t="s">
+      <c r="D185" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="E176" s="30" t="s">
+      <c r="E185" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F176" s="30">
+      <c r="F185" s="30">
         <v>1</v>
       </c>
-      <c r="G176" s="30">
+      <c r="G185" s="30">
         <v>350</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A177" s="40" t="s">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A186" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="B177" s="40" t="s">
+      <c r="B186" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="C177" s="41" t="s">
+      <c r="C186" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="D177" s="42" t="s">
+      <c r="D186" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="E177" s="30" t="s">
+      <c r="E186" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="F177" s="30">
+      <c r="F186" s="30">
         <v>351</v>
       </c>
-      <c r="G177" s="30">
+      <c r="G186" s="30">
         <v>10859</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A178" s="32" t="s">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A187" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B178" s="32" t="s">
+      <c r="B187" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="C178" s="33" t="s">
+      <c r="C187" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="D178" s="30" t="s">
+      <c r="D187" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="E178" s="30" t="s">
+      <c r="E187" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="F178" s="30">
+      <c r="F187" s="30">
         <v>1</v>
       </c>
-      <c r="G178" s="30">
+      <c r="G187" s="30">
         <v>18554</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A179" s="43" t="s">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A188" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="B179" s="32" t="s">
+      <c r="B188" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="C179" s="33" t="s">
+      <c r="C188" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="D179" s="30" t="s">
+      <c r="D188" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="E179" s="30" t="s">
+      <c r="E188" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F179" s="30">
+      <c r="F188" s="30">
         <v>1</v>
       </c>
-      <c r="G179" s="30">
+      <c r="G188" s="30">
         <v>199</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A180" s="43" t="s">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A189" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="B180" s="32" t="s">
+      <c r="B189" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="C180" s="33" t="s">
+      <c r="C189" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="D180" s="30" t="s">
+      <c r="D189" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="E180" s="30" t="s">
+      <c r="E189" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="F180" s="30">
+      <c r="F189" s="30">
         <v>200</v>
       </c>
-      <c r="G180" s="30">
+      <c r="G189" s="30">
         <v>17905</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A181" s="43" t="s">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A190" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="B181" s="32" t="s">
+      <c r="B190" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="C181" s="33" t="s">
+      <c r="C190" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="D181" s="30" t="s">
+      <c r="D190" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="E181" s="30" t="s">
+      <c r="E190" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F181" s="30">
+      <c r="F190" s="30">
         <v>17906</v>
       </c>
-      <c r="G181" s="30">
+      <c r="G190" s="30">
         <v>18554</v>
-      </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A182" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="B182" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="C182" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="D182" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="E182" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="F182" s="30">
-        <v>1</v>
-      </c>
-      <c r="G182" s="30">
-        <v>12573</v>
-      </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A183" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="B183" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="C183" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="D183" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="E183" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="F183" s="30">
-        <v>1</v>
-      </c>
-      <c r="G183" s="30">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A184" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="B184" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="C184" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="D184" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="E184" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F184" s="30">
-        <v>386</v>
-      </c>
-      <c r="G184" s="30">
-        <v>12352</v>
-      </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A185" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="B185" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="C185" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="D185" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="E185" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="F185" s="30">
-        <v>386</v>
-      </c>
-      <c r="G185" s="30">
-        <v>3583</v>
-      </c>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A186" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="B186" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="C186" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="D186" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="E186" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="F186" s="30">
-        <v>386</v>
-      </c>
-      <c r="G186" s="30">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A187" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="B187" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="C187" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="D187" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="E187" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="F187" s="30">
-        <v>890</v>
-      </c>
-      <c r="G187" s="30">
-        <v>1195</v>
-      </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A188" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="B188" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="C188" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="D188" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="E188" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="F188" s="30">
-        <v>1196</v>
-      </c>
-      <c r="G188" s="30">
-        <v>1876</v>
-      </c>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A189" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="B189" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="C189" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="D189" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="E189" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="F189" s="30">
-        <v>1877</v>
-      </c>
-      <c r="G189" s="30">
-        <v>2461</v>
-      </c>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A190" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="B190" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="C190" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="D190" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="E190" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="F190" s="30">
-        <v>2462</v>
-      </c>
-      <c r="G190" s="30">
-        <v>3583</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.2">
@@ -10578,13 +10587,13 @@
         <v>134</v>
       </c>
       <c r="E191" s="30" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F191" s="30">
-        <v>3584</v>
+        <v>1</v>
       </c>
       <c r="G191" s="30">
-        <v>3793</v>
+        <v>12573</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.2">
@@ -10601,13 +10610,13 @@
         <v>134</v>
       </c>
       <c r="E192" s="30" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F192" s="30">
-        <v>3794</v>
+        <v>1</v>
       </c>
       <c r="G192" s="30">
-        <v>7471</v>
+        <v>385</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.2">
@@ -10624,13 +10633,13 @@
         <v>134</v>
       </c>
       <c r="E193" s="30" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="F193" s="30">
-        <v>7472</v>
+        <v>386</v>
       </c>
       <c r="G193" s="30">
-        <v>7663</v>
+        <v>12352</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.2">
@@ -10647,13 +10656,13 @@
         <v>134</v>
       </c>
       <c r="E194" s="30" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="F194" s="30">
-        <v>7664</v>
+        <v>386</v>
       </c>
       <c r="G194" s="30">
-        <v>8704</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.2">
@@ -10670,13 +10679,13 @@
         <v>134</v>
       </c>
       <c r="E195" s="30" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="F195" s="30">
-        <v>8705</v>
+        <v>386</v>
       </c>
       <c r="G195" s="30">
-        <v>12349</v>
+        <v>889</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.2">
@@ -10693,13 +10702,13 @@
         <v>134</v>
       </c>
       <c r="E196" s="30" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="F196" s="30">
-        <v>8705</v>
+        <v>890</v>
       </c>
       <c r="G196" s="30">
-        <v>10192</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.2">
@@ -10716,13 +10725,13 @@
         <v>134</v>
       </c>
       <c r="E197" s="30" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F197" s="30">
-        <v>10193</v>
+        <v>1196</v>
       </c>
       <c r="G197" s="30">
-        <v>12349</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.2">
@@ -10739,433 +10748,450 @@
         <v>134</v>
       </c>
       <c r="E198" s="30" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="F198" s="30">
-        <v>12360</v>
+        <v>1877</v>
       </c>
       <c r="G198" s="30">
-        <v>12573</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199" s="44" t="s">
-        <v>138</v>
+        <v>35</v>
       </c>
       <c r="B199" s="44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C199" s="44" t="s">
         <v>27</v>
       </c>
       <c r="D199" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E199" s="30" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F199" s="30">
-        <v>1</v>
+        <v>2462</v>
       </c>
       <c r="G199" s="30">
-        <v>12983</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200" s="44" t="s">
-        <v>138</v>
+        <v>35</v>
       </c>
       <c r="B200" s="44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C200" s="44" t="s">
         <v>27</v>
       </c>
       <c r="D200" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E200" s="30" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="F200" s="30">
-        <v>499</v>
+        <v>3584</v>
       </c>
       <c r="G200" s="30">
-        <v>12480</v>
+        <v>3793</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201" s="44" t="s">
-        <v>138</v>
+        <v>35</v>
       </c>
       <c r="B201" s="44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C201" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="D201" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="E201" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="F201" s="17">
-        <v>2311</v>
-      </c>
-      <c r="G201" s="17">
-        <v>2904</v>
+      <c r="D201" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="E201" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F201" s="30">
+        <v>3794</v>
+      </c>
+      <c r="G201" s="30">
+        <v>7471</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202" s="44" t="s">
-        <v>138</v>
+        <v>35</v>
       </c>
       <c r="B202" s="44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C202" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="D202" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="E202" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="F202" s="17">
-        <v>2905</v>
-      </c>
-      <c r="G202" s="17">
-        <v>4035</v>
+      <c r="D202" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="E202" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F202" s="30">
+        <v>7472</v>
+      </c>
+      <c r="G202" s="30">
+        <v>7663</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203" s="44" t="s">
-        <v>140</v>
+        <v>35</v>
       </c>
       <c r="B203" s="44" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C203" s="44" t="s">
         <v>27</v>
       </c>
       <c r="D203" s="30" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E203" s="30" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="F203" s="30">
-        <v>1</v>
+        <v>7664</v>
       </c>
       <c r="G203" s="30">
-        <v>11276</v>
+        <v>8704</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204" s="44" t="s">
-        <v>140</v>
+        <v>35</v>
       </c>
       <c r="B204" s="44" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C204" s="44" t="s">
         <v>27</v>
       </c>
       <c r="D204" s="30" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E204" s="30" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="F204" s="30">
-        <v>124</v>
+        <v>8705</v>
       </c>
       <c r="G204" s="30">
-        <v>11031</v>
+        <v>12349</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205" s="44" t="s">
-        <v>140</v>
+        <v>35</v>
       </c>
       <c r="B205" s="44" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C205" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="D205" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="E205" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="F205" s="17">
-        <v>1627</v>
-      </c>
-      <c r="G205" s="17">
-        <v>2223</v>
+      <c r="D205" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="E205" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F205" s="30">
+        <v>8705</v>
+      </c>
+      <c r="G205" s="30">
+        <v>10192</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206" s="44" t="s">
-        <v>140</v>
+        <v>35</v>
       </c>
       <c r="B206" s="44" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C206" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="D206" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="E206" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="F206" s="17">
-        <v>2224</v>
-      </c>
-      <c r="G206" s="17">
-        <v>2943</v>
+      <c r="D206" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="E206" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F206" s="30">
+        <v>10193</v>
+      </c>
+      <c r="G206" s="30">
+        <v>12349</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207" s="44" t="s">
-        <v>139</v>
+        <v>35</v>
       </c>
       <c r="B207" s="44" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C207" s="44" t="s">
         <v>27</v>
       </c>
       <c r="D207" s="30" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E207" s="30" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
       <c r="F207" s="30">
-        <v>1</v>
+        <v>12360</v>
       </c>
       <c r="G207" s="30">
-        <v>7797</v>
+        <v>12573</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208" s="44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B208" s="44" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C208" s="44" t="s">
         <v>27</v>
       </c>
       <c r="D208" s="30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E208" s="30" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="F208" s="30">
         <v>1</v>
       </c>
       <c r="G208" s="30">
-        <v>7770</v>
+        <v>12983</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A209" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B209" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="C209" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="D209" s="30"/>
+      <c r="A209" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="B209" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="C209" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D209" s="30" t="s">
+        <v>135</v>
+      </c>
       <c r="E209" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="F209" s="30">
+        <v>499</v>
+      </c>
+      <c r="G209" s="30">
+        <v>12480</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A210" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="B210" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="C210" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D210" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E210" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F210" s="17">
+        <v>2311</v>
+      </c>
+      <c r="G210" s="17">
+        <v>2904</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A211" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="B211" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="C211" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D211" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E211" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F211" s="17">
+        <v>2905</v>
+      </c>
+      <c r="G211" s="17">
+        <v>4035</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A212" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="B212" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="C212" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D212" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="E212" s="30" t="s">
         <v>72</v>
-      </c>
-      <c r="F209" s="30">
-        <v>1</v>
-      </c>
-      <c r="G209" s="30">
-        <v>10053</v>
-      </c>
-    </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A210" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B210" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="C210" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="D210" s="30"/>
-      <c r="E210" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F210" s="30">
-        <v>1</v>
-      </c>
-      <c r="G210" s="30">
-        <v>10053</v>
-      </c>
-    </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A211" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B211" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="C211" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="D211" s="30"/>
-      <c r="E211" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="F211" s="30">
-        <v>1</v>
-      </c>
-      <c r="G211" s="30">
-        <v>2358</v>
-      </c>
-      <c r="H211" s="16"/>
-    </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A212" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B212" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="C212" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="D212" s="30"/>
-      <c r="E212" s="30" t="s">
-        <v>82</v>
       </c>
       <c r="F212" s="30">
         <v>1</v>
       </c>
       <c r="G212" s="30">
-        <v>345</v>
+        <v>11276</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A213" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B213" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="C213" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="D213" s="30"/>
+      <c r="A213" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="B213" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="C213" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D213" s="30" t="s">
+        <v>136</v>
+      </c>
       <c r="E213" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F213" s="30">
-        <v>346</v>
+        <v>124</v>
       </c>
       <c r="G213" s="30">
-        <v>852</v>
+        <v>11031</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A214" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B214" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="C214" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="D214" s="30"/>
-      <c r="E214" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="F214" s="30">
-        <v>655</v>
-      </c>
-      <c r="G214" s="30">
-        <v>852</v>
+      <c r="A214" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="B214" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="C214" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D214" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="E214" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F214" s="17">
+        <v>1627</v>
+      </c>
+      <c r="G214" s="17">
+        <v>2223</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A215" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B215" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="C215" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="D215" s="30"/>
-      <c r="E215" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="F215" s="30">
-        <v>853</v>
-      </c>
-      <c r="G215" s="30">
-        <v>2358</v>
+      <c r="A215" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="B215" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="C215" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D215" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="E215" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F215" s="17">
+        <v>2224</v>
+      </c>
+      <c r="G215" s="17">
+        <v>2943</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A216" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B216" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="C216" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="D216" s="30"/>
+      <c r="A216" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="B216" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="C216" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D216" s="30" t="s">
+        <v>137</v>
+      </c>
       <c r="E216" s="30" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="F216" s="30">
-        <v>2359</v>
+        <v>1</v>
       </c>
       <c r="G216" s="30">
-        <v>10050</v>
+        <v>7797</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A217" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B217" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="C217" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="D217" s="30"/>
+      <c r="A217" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="B217" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="C217" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D217" s="30" t="s">
+        <v>137</v>
+      </c>
       <c r="E217" s="30" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="F217" s="30">
-        <v>2359</v>
+        <v>1</v>
       </c>
       <c r="G217" s="30">
-        <v>3390</v>
+        <v>7770</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.2">
@@ -11180,13 +11206,13 @@
       </c>
       <c r="D218" s="30"/>
       <c r="E218" s="30" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="F218" s="30">
-        <v>3391</v>
+        <v>1</v>
       </c>
       <c r="G218" s="30">
-        <v>3978</v>
+        <v>10053</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.2">
@@ -11201,13 +11227,13 @@
       </c>
       <c r="D219" s="30"/>
       <c r="E219" s="30" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="F219" s="30">
-        <v>3979</v>
+        <v>1</v>
       </c>
       <c r="G219" s="30">
-        <v>4431</v>
+        <v>10053</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.2">
@@ -11222,14 +11248,15 @@
       </c>
       <c r="D220" s="30"/>
       <c r="E220" s="30" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="F220" s="30">
-        <v>4432</v>
+        <v>1</v>
       </c>
       <c r="G220" s="30">
-        <v>6303</v>
-      </c>
+        <v>2358</v>
+      </c>
+      <c r="H220" s="16"/>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" s="30" t="s">
@@ -11243,13 +11270,13 @@
       </c>
       <c r="D221" s="30"/>
       <c r="E221" s="30" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F221" s="30">
-        <v>6304</v>
+        <v>1</v>
       </c>
       <c r="G221" s="30">
-        <v>6687</v>
+        <v>345</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.2">
@@ -11264,13 +11291,13 @@
       </c>
       <c r="D222" s="30"/>
       <c r="E222" s="30" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="F222" s="30">
-        <v>6688</v>
+        <v>346</v>
       </c>
       <c r="G222" s="30">
-        <v>6762</v>
+        <v>852</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.2">
@@ -11285,13 +11312,13 @@
       </c>
       <c r="D223" s="30"/>
       <c r="E223" s="30" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="F223" s="30">
-        <v>6763</v>
+        <v>655</v>
       </c>
       <c r="G223" s="30">
-        <v>7557</v>
+        <v>852</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.2">
@@ -11306,95 +11333,203 @@
       </c>
       <c r="D224" s="30"/>
       <c r="E224" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="F224" s="30">
+        <v>853</v>
+      </c>
+      <c r="G224" s="30">
+        <v>2358</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A225" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B225" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C225" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D225" s="30"/>
+      <c r="E225" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="F225" s="30">
+        <v>2359</v>
+      </c>
+      <c r="G225" s="30">
+        <v>10050</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A226" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B226" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C226" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D226" s="30"/>
+      <c r="E226" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F226" s="30">
+        <v>2359</v>
+      </c>
+      <c r="G226" s="30">
+        <v>3390</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A227" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B227" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C227" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D227" s="30"/>
+      <c r="E227" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="F227" s="30">
+        <v>3391</v>
+      </c>
+      <c r="G227" s="30">
+        <v>3978</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A228" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B228" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C228" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D228" s="30"/>
+      <c r="E228" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="F228" s="30">
+        <v>3979</v>
+      </c>
+      <c r="G228" s="30">
+        <v>4431</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A229" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B229" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C229" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D229" s="30"/>
+      <c r="E229" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F229" s="30">
+        <v>4432</v>
+      </c>
+      <c r="G229" s="30">
+        <v>6303</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A230" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B230" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C230" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D230" s="30"/>
+      <c r="E230" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="F230" s="30">
+        <v>6304</v>
+      </c>
+      <c r="G230" s="30">
+        <v>6687</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A231" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B231" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C231" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D231" s="30"/>
+      <c r="E231" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F231" s="30">
+        <v>6688</v>
+      </c>
+      <c r="G231" s="30">
+        <v>6762</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A232" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B232" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C232" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D232" s="30"/>
+      <c r="E232" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="F232" s="30">
+        <v>6763</v>
+      </c>
+      <c r="G232" s="30">
+        <v>7557</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A233" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B233" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C233" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D233" s="30"/>
+      <c r="E233" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="F224" s="30">
+      <c r="F233" s="30">
         <v>7558</v>
       </c>
-      <c r="G224" s="30">
+      <c r="G233" s="30">
         <v>10050</v>
       </c>
-    </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A225" s="47"/>
-      <c r="B225" s="47"/>
-      <c r="C225" s="48"/>
-      <c r="D225" s="48"/>
-      <c r="E225" s="47"/>
-      <c r="F225" s="47"/>
-      <c r="G225" s="47"/>
-    </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A226" s="47"/>
-      <c r="B226" s="47"/>
-      <c r="C226" s="48"/>
-      <c r="D226" s="48"/>
-      <c r="E226" s="47"/>
-      <c r="F226" s="47"/>
-      <c r="G226" s="47"/>
-    </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A227" s="47"/>
-      <c r="B227" s="47"/>
-      <c r="C227" s="48"/>
-      <c r="D227" s="48"/>
-      <c r="E227" s="47"/>
-      <c r="F227" s="47"/>
-      <c r="G227" s="47"/>
-    </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A228" s="47"/>
-      <c r="B228" s="47"/>
-      <c r="C228" s="48"/>
-      <c r="D228" s="48"/>
-      <c r="E228" s="47"/>
-      <c r="F228" s="47"/>
-      <c r="G228" s="47"/>
-    </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A229" s="47"/>
-      <c r="B229" s="47"/>
-      <c r="C229" s="48"/>
-      <c r="D229" s="48"/>
-      <c r="E229" s="47"/>
-      <c r="F229" s="47"/>
-      <c r="G229" s="47"/>
-    </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A230" s="47"/>
-      <c r="B230" s="47"/>
-      <c r="C230" s="48"/>
-      <c r="D230" s="48"/>
-      <c r="E230" s="47"/>
-      <c r="F230" s="47"/>
-      <c r="G230" s="47"/>
-    </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A231" s="47"/>
-      <c r="B231" s="47"/>
-      <c r="C231" s="48"/>
-      <c r="D231" s="48"/>
-      <c r="E231" s="47"/>
-      <c r="F231" s="47"/>
-      <c r="G231" s="47"/>
-    </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A232" s="47"/>
-      <c r="B232" s="47"/>
-      <c r="C232" s="48"/>
-      <c r="D232" s="48"/>
-      <c r="E232" s="47"/>
-      <c r="F232" s="47"/>
-      <c r="G232" s="47"/>
-    </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A233" s="47"/>
-      <c r="B233" s="47"/>
-      <c r="C233" s="48"/>
-      <c r="D233" s="48"/>
-      <c r="E233" s="47"/>
-      <c r="F233" s="47"/>
-      <c r="G233" s="47"/>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A234" s="47"/>
@@ -11569,8 +11704,8 @@
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A253" s="47"/>
-      <c r="B253" s="49"/>
-      <c r="C253" s="50"/>
+      <c r="B253" s="47"/>
+      <c r="C253" s="48"/>
       <c r="D253" s="48"/>
       <c r="E253" s="47"/>
       <c r="F253" s="47"/>
@@ -11578,72 +11713,72 @@
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A254" s="47"/>
-      <c r="B254" s="49"/>
-      <c r="C254" s="50"/>
-      <c r="D254" s="50"/>
+      <c r="B254" s="47"/>
+      <c r="C254" s="48"/>
+      <c r="D254" s="48"/>
       <c r="E254" s="47"/>
       <c r="F254" s="47"/>
       <c r="G254" s="47"/>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A255" s="47"/>
-      <c r="B255" s="49"/>
-      <c r="C255" s="50"/>
-      <c r="D255" s="50"/>
+      <c r="B255" s="47"/>
+      <c r="C255" s="48"/>
+      <c r="D255" s="48"/>
       <c r="E255" s="47"/>
       <c r="F255" s="47"/>
       <c r="G255" s="47"/>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A256" s="47"/>
-      <c r="B256" s="49"/>
-      <c r="C256" s="50"/>
-      <c r="D256" s="50"/>
+      <c r="B256" s="47"/>
+      <c r="C256" s="48"/>
+      <c r="D256" s="48"/>
       <c r="E256" s="47"/>
       <c r="F256" s="47"/>
       <c r="G256" s="47"/>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A257" s="47"/>
-      <c r="B257" s="49"/>
-      <c r="C257" s="50"/>
-      <c r="D257" s="50"/>
+      <c r="B257" s="47"/>
+      <c r="C257" s="48"/>
+      <c r="D257" s="48"/>
       <c r="E257" s="47"/>
       <c r="F257" s="47"/>
       <c r="G257" s="47"/>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A258" s="47"/>
-      <c r="B258" s="49"/>
-      <c r="C258" s="50"/>
-      <c r="D258" s="50"/>
+      <c r="B258" s="47"/>
+      <c r="C258" s="48"/>
+      <c r="D258" s="48"/>
       <c r="E258" s="47"/>
       <c r="F258" s="47"/>
       <c r="G258" s="47"/>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A259" s="47"/>
-      <c r="B259" s="49"/>
-      <c r="C259" s="50"/>
-      <c r="D259" s="50"/>
+      <c r="B259" s="47"/>
+      <c r="C259" s="48"/>
+      <c r="D259" s="48"/>
       <c r="E259" s="47"/>
       <c r="F259" s="47"/>
       <c r="G259" s="47"/>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260" s="47"/>
-      <c r="B260" s="49"/>
-      <c r="C260" s="50"/>
-      <c r="D260" s="50"/>
+      <c r="B260" s="47"/>
+      <c r="C260" s="48"/>
+      <c r="D260" s="48"/>
       <c r="E260" s="47"/>
       <c r="F260" s="47"/>
       <c r="G260" s="47"/>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A261" s="47"/>
-      <c r="B261" s="49"/>
-      <c r="C261" s="50"/>
-      <c r="D261" s="50"/>
+      <c r="B261" s="47"/>
+      <c r="C261" s="48"/>
+      <c r="D261" s="48"/>
       <c r="E261" s="47"/>
       <c r="F261" s="47"/>
       <c r="G261" s="47"/>
@@ -11652,7 +11787,7 @@
       <c r="A262" s="47"/>
       <c r="B262" s="49"/>
       <c r="C262" s="50"/>
-      <c r="D262" s="50"/>
+      <c r="D262" s="48"/>
       <c r="E262" s="47"/>
       <c r="F262" s="47"/>
       <c r="G262" s="47"/>
@@ -11786,7 +11921,7 @@
     <row r="277" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A277" s="47"/>
       <c r="B277" s="49"/>
-      <c r="C277" s="48"/>
+      <c r="C277" s="50"/>
       <c r="D277" s="50"/>
       <c r="E277" s="47"/>
       <c r="F277" s="47"/>
@@ -11796,7 +11931,7 @@
       <c r="A278" s="47"/>
       <c r="B278" s="49"/>
       <c r="C278" s="50"/>
-      <c r="D278" s="48"/>
+      <c r="D278" s="50"/>
       <c r="E278" s="47"/>
       <c r="F278" s="47"/>
       <c r="G278" s="47"/>
@@ -11857,8 +11992,8 @@
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A285" s="47"/>
-      <c r="B285" s="47"/>
-      <c r="C285" s="48"/>
+      <c r="B285" s="49"/>
+      <c r="C285" s="50"/>
       <c r="D285" s="50"/>
       <c r="E285" s="47"/>
       <c r="F285" s="47"/>
@@ -11866,17 +12001,17 @@
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A286" s="47"/>
-      <c r="B286" s="47"/>
+      <c r="B286" s="49"/>
       <c r="C286" s="48"/>
-      <c r="D286" s="48"/>
+      <c r="D286" s="50"/>
       <c r="E286" s="47"/>
       <c r="F286" s="47"/>
       <c r="G286" s="47"/>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A287" s="47"/>
-      <c r="B287" s="47"/>
-      <c r="C287" s="48"/>
+      <c r="B287" s="49"/>
+      <c r="C287" s="50"/>
       <c r="D287" s="48"/>
       <c r="E287" s="47"/>
       <c r="F287" s="47"/>
@@ -11884,54 +12019,54 @@
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A288" s="47"/>
-      <c r="B288" s="47"/>
-      <c r="C288" s="48"/>
-      <c r="D288" s="48"/>
+      <c r="B288" s="49"/>
+      <c r="C288" s="50"/>
+      <c r="D288" s="50"/>
       <c r="E288" s="47"/>
       <c r="F288" s="47"/>
       <c r="G288" s="47"/>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A289" s="47"/>
-      <c r="B289" s="47"/>
-      <c r="C289" s="48"/>
-      <c r="D289" s="48"/>
+      <c r="B289" s="49"/>
+      <c r="C289" s="50"/>
+      <c r="D289" s="50"/>
       <c r="E289" s="47"/>
       <c r="F289" s="47"/>
       <c r="G289" s="47"/>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A290" s="47"/>
-      <c r="B290" s="47"/>
-      <c r="C290" s="48"/>
-      <c r="D290" s="48"/>
+      <c r="B290" s="49"/>
+      <c r="C290" s="50"/>
+      <c r="D290" s="50"/>
       <c r="E290" s="47"/>
       <c r="F290" s="47"/>
       <c r="G290" s="47"/>
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A291" s="47"/>
-      <c r="B291" s="47"/>
-      <c r="C291" s="48"/>
-      <c r="D291" s="48"/>
+      <c r="B291" s="49"/>
+      <c r="C291" s="50"/>
+      <c r="D291" s="50"/>
       <c r="E291" s="47"/>
       <c r="F291" s="47"/>
       <c r="G291" s="47"/>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A292" s="47"/>
-      <c r="B292" s="47"/>
-      <c r="C292" s="48"/>
-      <c r="D292" s="48"/>
+      <c r="B292" s="49"/>
+      <c r="C292" s="50"/>
+      <c r="D292" s="50"/>
       <c r="E292" s="47"/>
       <c r="F292" s="47"/>
       <c r="G292" s="47"/>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A293" s="47"/>
-      <c r="B293" s="47"/>
-      <c r="C293" s="48"/>
-      <c r="D293" s="48"/>
+      <c r="B293" s="49"/>
+      <c r="C293" s="50"/>
+      <c r="D293" s="50"/>
       <c r="E293" s="47"/>
       <c r="F293" s="47"/>
       <c r="G293" s="47"/>
@@ -11940,7 +12075,7 @@
       <c r="A294" s="47"/>
       <c r="B294" s="47"/>
       <c r="C294" s="48"/>
-      <c r="D294" s="48"/>
+      <c r="D294" s="50"/>
       <c r="E294" s="47"/>
       <c r="F294" s="47"/>
       <c r="G294" s="47"/>
@@ -11981,117 +12116,158 @@
       <c r="F298" s="47"/>
       <c r="G298" s="47"/>
     </row>
-    <row r="967" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C967"/>
-      <c r="D967"/>
-      <c r="E967" s="1"/>
-    </row>
-    <row r="1103" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1103" s="1"/>
-      <c r="C1103"/>
-      <c r="D1103"/>
-    </row>
-    <row r="1104" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1104" s="1"/>
-      <c r="C1104"/>
-      <c r="D1104"/>
-    </row>
-    <row r="1229" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1229" s="1"/>
-      <c r="C1229"/>
-      <c r="D1229"/>
-    </row>
-    <row r="1230" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1230" s="1"/>
-      <c r="C1230"/>
-      <c r="D1230"/>
-    </row>
-    <row r="1231" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1231" s="1"/>
-      <c r="C1231"/>
-      <c r="D1231"/>
-    </row>
-    <row r="1232" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1232" s="1"/>
-      <c r="C1232"/>
-      <c r="D1232"/>
-    </row>
-    <row r="1233" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1233" s="1"/>
-      <c r="C1233"/>
-      <c r="D1233"/>
-    </row>
-    <row r="1234" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1234" s="1"/>
-      <c r="C1234"/>
-      <c r="D1234"/>
-    </row>
-    <row r="1279" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E1279" s="1"/>
-      <c r="F1279" s="1"/>
-    </row>
-    <row r="1280" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E1280" s="1"/>
-      <c r="F1280" s="1"/>
-    </row>
-    <row r="1281" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E1281" s="1"/>
-      <c r="F1281" s="1"/>
-    </row>
-    <row r="1283" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1283" s="1"/>
-    </row>
-    <row r="1284" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1284" s="1"/>
-    </row>
-    <row r="1285" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1285" s="1"/>
-    </row>
-    <row r="1286" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1286" s="1"/>
-    </row>
-    <row r="1287" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1287" s="1"/>
-    </row>
-    <row r="1306" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1306" s="1"/>
-      <c r="C1306"/>
-      <c r="D1306"/>
-    </row>
-    <row r="1307" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1307" s="1"/>
-      <c r="C1307"/>
-      <c r="D1307"/>
-    </row>
-    <row r="1308" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1308" s="1"/>
-      <c r="C1308"/>
-      <c r="D1308"/>
-    </row>
-    <row r="1309" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1309" s="1"/>
-      <c r="C1309"/>
-      <c r="D1309"/>
-    </row>
-    <row r="1310" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1310" s="1"/>
-      <c r="C1310"/>
-      <c r="D1310"/>
-    </row>
-    <row r="1311" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1311" s="1"/>
-      <c r="C1311"/>
-      <c r="D1311"/>
-    </row>
-    <row r="1312" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1312" s="1"/>
-      <c r="C1312"/>
-      <c r="D1312"/>
-    </row>
-    <row r="1314" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1314" s="1"/>
-      <c r="C1314"/>
-      <c r="D1314"/>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A299" s="47"/>
+      <c r="B299" s="47"/>
+      <c r="C299" s="48"/>
+      <c r="D299" s="48"/>
+      <c r="E299" s="47"/>
+      <c r="F299" s="47"/>
+      <c r="G299" s="47"/>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A300" s="47"/>
+      <c r="B300" s="47"/>
+      <c r="C300" s="48"/>
+      <c r="D300" s="48"/>
+      <c r="E300" s="47"/>
+      <c r="F300" s="47"/>
+      <c r="G300" s="47"/>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A301" s="47"/>
+      <c r="B301" s="47"/>
+      <c r="C301" s="48"/>
+      <c r="D301" s="48"/>
+      <c r="E301" s="47"/>
+      <c r="F301" s="47"/>
+      <c r="G301" s="47"/>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A302" s="47"/>
+      <c r="B302" s="47"/>
+      <c r="C302" s="48"/>
+      <c r="D302" s="48"/>
+      <c r="E302" s="47"/>
+      <c r="F302" s="47"/>
+      <c r="G302" s="47"/>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A303" s="47"/>
+      <c r="B303" s="47"/>
+      <c r="C303" s="48"/>
+      <c r="D303" s="48"/>
+      <c r="E303" s="47"/>
+      <c r="F303" s="47"/>
+      <c r="G303" s="47"/>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A304" s="47"/>
+      <c r="B304" s="47"/>
+      <c r="C304" s="48"/>
+      <c r="D304" s="48"/>
+      <c r="E304" s="47"/>
+      <c r="F304" s="47"/>
+      <c r="G304" s="47"/>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A305" s="47"/>
+      <c r="B305" s="47"/>
+      <c r="C305" s="48"/>
+      <c r="D305" s="48"/>
+      <c r="E305" s="47"/>
+      <c r="F305" s="47"/>
+      <c r="G305" s="47"/>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A306" s="47"/>
+      <c r="B306" s="47"/>
+      <c r="C306" s="48"/>
+      <c r="D306" s="48"/>
+      <c r="E306" s="47"/>
+      <c r="F306" s="47"/>
+      <c r="G306" s="47"/>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A307" s="47"/>
+      <c r="B307" s="47"/>
+      <c r="C307" s="48"/>
+      <c r="D307" s="48"/>
+      <c r="E307" s="47"/>
+      <c r="F307" s="47"/>
+      <c r="G307" s="47"/>
+    </row>
+    <row r="976" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C976"/>
+      <c r="D976"/>
+      <c r="E976" s="1"/>
+    </row>
+    <row r="1112" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1112" s="1"/>
+      <c r="C1112"/>
+      <c r="D1112"/>
+    </row>
+    <row r="1113" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1113" s="1"/>
+      <c r="C1113"/>
+      <c r="D1113"/>
+    </row>
+    <row r="1238" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1238" s="1"/>
+      <c r="C1238"/>
+      <c r="D1238"/>
+    </row>
+    <row r="1239" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1239" s="1"/>
+      <c r="C1239"/>
+      <c r="D1239"/>
+    </row>
+    <row r="1240" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1240" s="1"/>
+      <c r="C1240"/>
+      <c r="D1240"/>
+    </row>
+    <row r="1241" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1241" s="1"/>
+      <c r="C1241"/>
+      <c r="D1241"/>
+    </row>
+    <row r="1242" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1242" s="1"/>
+      <c r="C1242"/>
+      <c r="D1242"/>
+    </row>
+    <row r="1243" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1243" s="1"/>
+      <c r="C1243"/>
+      <c r="D1243"/>
+    </row>
+    <row r="1288" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E1288" s="1"/>
+      <c r="F1288" s="1"/>
+    </row>
+    <row r="1289" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E1289" s="1"/>
+      <c r="F1289" s="1"/>
+    </row>
+    <row r="1290" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E1290" s="1"/>
+      <c r="F1290" s="1"/>
+    </row>
+    <row r="1292" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1292" s="1"/>
+    </row>
+    <row r="1293" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1293" s="1"/>
+    </row>
+    <row r="1294" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1294" s="1"/>
+    </row>
+    <row r="1295" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1295" s="1"/>
+    </row>
+    <row r="1296" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1296" s="1"/>
     </row>
     <row r="1315" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1315" s="1"/>
@@ -12118,126 +12294,166 @@
       <c r="C1319"/>
       <c r="D1319"/>
     </row>
-    <row r="1371" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1371" s="1"/>
-      <c r="C1371"/>
-      <c r="D1371"/>
-    </row>
-    <row r="1372" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1372" s="1"/>
-      <c r="C1372"/>
-      <c r="D1372"/>
-    </row>
-    <row r="1373" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1373" s="1"/>
-      <c r="C1373"/>
-      <c r="D1373"/>
-    </row>
-    <row r="1374" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1374" s="1"/>
-      <c r="C1374"/>
-      <c r="D1374"/>
-    </row>
-    <row r="1376" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1376" s="1"/>
-      <c r="C1376"/>
-      <c r="D1376"/>
-    </row>
-    <row r="1377" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1377" s="1"/>
-      <c r="C1377"/>
-      <c r="D1377"/>
-    </row>
-    <row r="1378" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1378" s="1"/>
-      <c r="C1378"/>
-      <c r="D1378"/>
-    </row>
-    <row r="1379" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1379" s="1"/>
-      <c r="C1379"/>
-      <c r="D1379"/>
-    </row>
-    <row r="1414" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1414" s="1"/>
-      <c r="C1414"/>
-      <c r="D1414"/>
-    </row>
-    <row r="1415" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1415" s="1"/>
-      <c r="C1415"/>
-      <c r="D1415"/>
-    </row>
-    <row r="1416" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1416" s="1"/>
-      <c r="C1416"/>
-      <c r="D1416"/>
-    </row>
-    <row r="1417" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1417" s="1"/>
-      <c r="C1417"/>
-      <c r="D1417"/>
-    </row>
-    <row r="1418" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1418" s="1"/>
-      <c r="C1418"/>
-      <c r="D1418"/>
-    </row>
-    <row r="1419" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1419" s="1"/>
-      <c r="C1419"/>
-      <c r="D1419"/>
-    </row>
-    <row r="1461" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E1461" s="1"/>
-      <c r="F1461" s="1"/>
-    </row>
-    <row r="1462" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C1462" s="3"/>
-      <c r="E1462" s="1"/>
-      <c r="F1462" s="1"/>
-    </row>
-    <row r="1463" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C1463" s="3"/>
-      <c r="D1463" s="3"/>
-      <c r="E1463" s="1"/>
-      <c r="F1463" s="1"/>
-    </row>
-    <row r="1464" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C1464" s="3"/>
-      <c r="D1464" s="3"/>
-      <c r="E1464" s="1"/>
-      <c r="F1464" s="1"/>
-    </row>
-    <row r="1465" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D1465" s="3"/>
-      <c r="E1465" s="1"/>
-      <c r="F1465" s="1"/>
-    </row>
-    <row r="1528" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1528" s="1"/>
-      <c r="C1528"/>
-      <c r="D1528"/>
-    </row>
-    <row r="1529" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1529" s="1"/>
-      <c r="C1529"/>
-      <c r="D1529"/>
-    </row>
-    <row r="1530" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1530" s="1"/>
-      <c r="C1530"/>
-      <c r="D1530"/>
-    </row>
-    <row r="1531" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1531" s="1"/>
-      <c r="C1531"/>
-      <c r="D1531"/>
+    <row r="1320" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1320" s="1"/>
+      <c r="C1320"/>
+      <c r="D1320"/>
+    </row>
+    <row r="1321" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1321" s="1"/>
+      <c r="C1321"/>
+      <c r="D1321"/>
+    </row>
+    <row r="1323" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1323" s="1"/>
+      <c r="C1323"/>
+      <c r="D1323"/>
+    </row>
+    <row r="1324" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1324" s="1"/>
+      <c r="C1324"/>
+      <c r="D1324"/>
+    </row>
+    <row r="1325" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1325" s="1"/>
+      <c r="C1325"/>
+      <c r="D1325"/>
+    </row>
+    <row r="1326" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1326" s="1"/>
+      <c r="C1326"/>
+      <c r="D1326"/>
+    </row>
+    <row r="1327" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1327" s="1"/>
+      <c r="C1327"/>
+      <c r="D1327"/>
+    </row>
+    <row r="1328" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1328" s="1"/>
+      <c r="C1328"/>
+      <c r="D1328"/>
+    </row>
+    <row r="1380" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1380" s="1"/>
+      <c r="C1380"/>
+      <c r="D1380"/>
+    </row>
+    <row r="1381" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1381" s="1"/>
+      <c r="C1381"/>
+      <c r="D1381"/>
+    </row>
+    <row r="1382" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1382" s="1"/>
+      <c r="C1382"/>
+      <c r="D1382"/>
+    </row>
+    <row r="1383" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1383" s="1"/>
+      <c r="C1383"/>
+      <c r="D1383"/>
+    </row>
+    <row r="1385" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1385" s="1"/>
+      <c r="C1385"/>
+      <c r="D1385"/>
+    </row>
+    <row r="1386" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1386" s="1"/>
+      <c r="C1386"/>
+      <c r="D1386"/>
+    </row>
+    <row r="1387" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1387" s="1"/>
+      <c r="C1387"/>
+      <c r="D1387"/>
+    </row>
+    <row r="1388" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1388" s="1"/>
+      <c r="C1388"/>
+      <c r="D1388"/>
+    </row>
+    <row r="1423" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1423" s="1"/>
+      <c r="C1423"/>
+      <c r="D1423"/>
+    </row>
+    <row r="1424" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1424" s="1"/>
+      <c r="C1424"/>
+      <c r="D1424"/>
+    </row>
+    <row r="1425" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1425" s="1"/>
+      <c r="C1425"/>
+      <c r="D1425"/>
+    </row>
+    <row r="1426" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1426" s="1"/>
+      <c r="C1426"/>
+      <c r="D1426"/>
+    </row>
+    <row r="1427" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1427" s="1"/>
+      <c r="C1427"/>
+      <c r="D1427"/>
+    </row>
+    <row r="1428" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1428" s="1"/>
+      <c r="C1428"/>
+      <c r="D1428"/>
+    </row>
+    <row r="1470" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="E1470" s="1"/>
+      <c r="F1470" s="1"/>
+    </row>
+    <row r="1471" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C1471" s="3"/>
+      <c r="E1471" s="1"/>
+      <c r="F1471" s="1"/>
+    </row>
+    <row r="1472" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C1472" s="3"/>
+      <c r="D1472" s="3"/>
+      <c r="E1472" s="1"/>
+      <c r="F1472" s="1"/>
+    </row>
+    <row r="1473" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C1473" s="3"/>
+      <c r="D1473" s="3"/>
+      <c r="E1473" s="1"/>
+      <c r="F1473" s="1"/>
+    </row>
+    <row r="1474" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D1474" s="3"/>
+      <c r="E1474" s="1"/>
+      <c r="F1474" s="1"/>
+    </row>
+    <row r="1537" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1537" s="1"/>
+      <c r="C1537"/>
+      <c r="D1537"/>
+    </row>
+    <row r="1538" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1538" s="1"/>
+      <c r="C1538"/>
+      <c r="D1538"/>
+    </row>
+    <row r="1539" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1539" s="1"/>
+      <c r="C1539"/>
+      <c r="D1539"/>
+    </row>
+    <row r="1540" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1540" s="1"/>
+      <c r="C1540"/>
+      <c r="D1540"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G224">
-    <sortCondition ref="C2:C224"/>
-    <sortCondition ref="D2:D224"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G233">
+    <sortCondition ref="C2:C233"/>
+    <sortCondition ref="D2:D233"/>
   </sortState>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>